<commit_message>
triple click selects a line
</commit_message>
<xml_diff>
--- a/FxEditor Feature Matrix.xlsx
+++ b/FxEditor Feature Matrix.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="218">
   <si>
     <t>Feature</t>
   </si>
@@ -669,6 +669,9 @@
   </si>
   <si>
     <t>shift right mouse click shows a popup menu</t>
+  </si>
+  <si>
+    <t>all but last line: line:0..(line+1):0, last line: line:0..line:max-1</t>
   </si>
 </sst>
 </file>
@@ -928,7 +931,7 @@
           <c:yMode val="edge"/>
           <c:x val="3.8461559098965002E-2"/>
           <c:y val="2.2690437601296611E-2"/>
-          <c:w val="0.91978071330955102"/>
+          <c:w val="0.91978071330955113"/>
           <c:h val="0.89627228525119951"/>
         </c:manualLayout>
       </c:layout>
@@ -1020,7 +1023,7 @@
                   <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>48</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1112,7 +1115,7 @@
                   <c:v>158</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>159</c:v>
+                  <c:v>158</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1308,11 +1311,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="122596736"/>
-        <c:axId val="122295424"/>
+        <c:axId val="166374784"/>
+        <c:axId val="166204544"/>
       </c:areaChart>
       <c:dateAx>
-        <c:axId val="122596736"/>
+        <c:axId val="166374784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1345,7 +1348,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="122295424"/>
+        <c:crossAx val="166204544"/>
         <c:crosses val="autoZero"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
@@ -1355,7 +1358,7 @@
         <c:minorTimeUnit val="months"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="122295424"/>
+        <c:axId val="166204544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1397,7 +1400,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="122596736"/>
+        <c:crossAx val="166374784"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1420,7 +1423,7 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="4.5828229804607823E-2"/>
-          <c:y val="0.33819556996218342"/>
+          <c:y val="0.33819556996218347"/>
           <c:w val="0.12857154394162268"/>
           <c:h val="0.11669367909238262"/>
         </c:manualLayout>
@@ -1487,7 +1490,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="1" l="0.75000000000001299" r="0.75000000000001299" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.7500000000000131" r="0.7500000000000131" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup paperSize="9" orientation="landscape" horizontalDpi="1200" verticalDpi="1200"/>
   </c:printSettings>
 </c:chartSpace>
@@ -1541,7 +1544,7 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="4.4510450248127477E-2"/>
+          <c:x val="4.4510450248127491E-2"/>
           <c:y val="0.10032394165889739"/>
           <c:w val="0.79228601441663349"/>
           <c:h val="0.79935527708863363"/>
@@ -1635,17 +1638,17 @@
                   <c:v>0.22966507177033493</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.23076923076923078</c:v>
+                  <c:v>0.23923444976076555</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="122327424"/>
-        <c:axId val="122328960"/>
+        <c:axId val="166228352"/>
+        <c:axId val="166229888"/>
       </c:areaChart>
       <c:dateAx>
-        <c:axId val="122327424"/>
+        <c:axId val="166228352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1653,13 +1656,13 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="yyyy\/mm\/dd" sourceLinked="1"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="122328960"/>
+        <c:crossAx val="166229888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="122328960"/>
+        <c:axId val="166229888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1702,7 +1705,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="122327424"/>
+        <c:crossAx val="166228352"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1751,7 +1754,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="1" l="0.75000000000001299" r="0.75000000000001299" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.7500000000000131" r="0.7500000000000131" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
   </c:printSettings>
 </c:chartSpace>
@@ -1861,7 +1864,7 @@
                   <c:v>158</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>159</c:v>
+                  <c:v>158</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1959,11 +1962,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="122349824"/>
-        <c:axId val="122351616"/>
+        <c:axId val="166250752"/>
+        <c:axId val="166256640"/>
       </c:areaChart>
       <c:dateAx>
-        <c:axId val="122349824"/>
+        <c:axId val="166250752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1996,7 +1999,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="122351616"/>
+        <c:crossAx val="166256640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
@@ -2005,7 +2008,7 @@
         <c:minorTimeUnit val="months"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="122351616"/>
+        <c:axId val="166256640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2047,7 +2050,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="122349824"/>
+        <c:crossAx val="166250752"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2096,7 +2099,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="1" l="0.75000000000001299" r="0.75000000000001299" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.7500000000000131" r="0.7500000000000131" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
   </c:printSettings>
 </c:chartSpace>
@@ -2554,10 +2557,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D373"/>
+  <dimension ref="A1:D374"/>
   <sheetViews>
-    <sheetView topLeftCell="A271" workbookViewId="0">
-      <selection activeCell="A265" sqref="A265:XFD268"/>
+    <sheetView topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="B129" sqref="B129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.5"/>
@@ -3538,50 +3541,50 @@
         <v>169</v>
       </c>
       <c r="C127" s="7" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="D127" s="4"/>
     </row>
     <row r="128" spans="2:4" s="6" customFormat="1">
-      <c r="B128" s="20"/>
-      <c r="C128" s="7"/>
+      <c r="B128" s="23" t="s">
+        <v>217</v>
+      </c>
+      <c r="C128" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="D128" s="4"/>
     </row>
     <row r="129" spans="2:4" s="6" customFormat="1">
-      <c r="B129" s="20" t="s">
+      <c r="B129" s="20"/>
+      <c r="C129" s="7"/>
+      <c r="D129" s="4"/>
+    </row>
+    <row r="130" spans="2:4" s="6" customFormat="1">
+      <c r="B130" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="C129" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D129" s="4"/>
-    </row>
-    <row r="130" spans="2:4" s="6" customFormat="1">
-      <c r="B130" s="23" t="s">
+      <c r="C130" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D130" s="4"/>
+    </row>
+    <row r="131" spans="2:4" s="6" customFormat="1">
+      <c r="B131" s="23" t="s">
         <v>215</v>
       </c>
-      <c r="C130" s="7" t="s">
+      <c r="C131" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D130" s="4"/>
-    </row>
-    <row r="131" spans="2:4" s="6" customFormat="1">
-      <c r="B131" s="22"/>
-      <c r="C131" s="7"/>
       <c r="D131" s="4"/>
     </row>
     <row r="132" spans="2:4" s="6" customFormat="1">
-      <c r="B132" s="20" t="s">
+      <c r="B132" s="22"/>
+      <c r="C132" s="7"/>
+      <c r="D132" s="4"/>
+    </row>
+    <row r="133" spans="2:4" s="6" customFormat="1">
+      <c r="B133" s="20" t="s">
         <v>64</v>
-      </c>
-      <c r="C132" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D132" s="4"/>
-    </row>
-    <row r="133" spans="2:4" s="6" customFormat="1">
-      <c r="B133" s="23" t="s">
-        <v>65</v>
       </c>
       <c r="C133" s="7" t="s">
         <v>14</v>
@@ -3590,30 +3593,30 @@
     </row>
     <row r="134" spans="2:4" s="6" customFormat="1">
       <c r="B134" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="C134" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D134" s="4"/>
+    </row>
+    <row r="135" spans="2:4" s="6" customFormat="1">
+      <c r="B135" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="C134" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D134" s="4"/>
-    </row>
-    <row r="135" spans="2:4" s="6" customFormat="1">
-      <c r="B135" s="20"/>
-      <c r="C135" s="7"/>
+      <c r="C135" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="D135" s="4"/>
     </row>
     <row r="136" spans="2:4" s="6" customFormat="1">
-      <c r="B136" s="20" t="s">
+      <c r="B136" s="20"/>
+      <c r="C136" s="7"/>
+      <c r="D136" s="4"/>
+    </row>
+    <row r="137" spans="2:4" s="6" customFormat="1">
+      <c r="B137" s="20" t="s">
         <v>68</v>
-      </c>
-      <c r="C136" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D136" s="4"/>
-    </row>
-    <row r="137" spans="2:4" s="6" customFormat="1">
-      <c r="B137" s="23" t="s">
-        <v>67</v>
       </c>
       <c r="C137" s="7" t="s">
         <v>2</v>
@@ -3622,53 +3625,53 @@
     </row>
     <row r="138" spans="2:4" s="6" customFormat="1">
       <c r="B138" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="C138" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D138" s="4"/>
+    </row>
+    <row r="139" spans="2:4" s="6" customFormat="1">
+      <c r="B139" s="23" t="s">
         <v>162</v>
       </c>
-      <c r="C138" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D138" s="4"/>
-    </row>
-    <row r="139" spans="2:4" s="6" customFormat="1">
-      <c r="B139" s="22"/>
-      <c r="C139" s="7"/>
+      <c r="C139" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="D139" s="4"/>
     </row>
     <row r="140" spans="2:4" s="6" customFormat="1">
-      <c r="B140" s="20" t="s">
+      <c r="B140" s="22"/>
+      <c r="C140" s="7"/>
+      <c r="D140" s="4"/>
+    </row>
+    <row r="141" spans="2:4" s="6" customFormat="1">
+      <c r="B141" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="C140" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D140" s="4"/>
-    </row>
-    <row r="141" spans="2:4" s="6" customFormat="1">
-      <c r="B141" s="23" t="s">
+      <c r="C141" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D141" s="4"/>
+    </row>
+    <row r="142" spans="2:4" s="6" customFormat="1">
+      <c r="B142" s="23" t="s">
         <v>76</v>
       </c>
-      <c r="C141" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D141" s="4"/>
-    </row>
-    <row r="142" spans="2:4" s="6" customFormat="1">
-      <c r="B142" s="22"/>
-      <c r="C142" s="7"/>
+      <c r="C142" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="D142" s="4"/>
     </row>
     <row r="143" spans="2:4" s="6" customFormat="1">
-      <c r="B143" s="20" t="s">
+      <c r="B143" s="22"/>
+      <c r="C143" s="7"/>
+      <c r="D143" s="4"/>
+    </row>
+    <row r="144" spans="2:4" s="6" customFormat="1">
+      <c r="B144" s="20" t="s">
         <v>73</v>
-      </c>
-      <c r="C143" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D143" s="4"/>
-    </row>
-    <row r="144" spans="2:4" s="6" customFormat="1">
-      <c r="B144" s="23" t="s">
-        <v>75</v>
       </c>
       <c r="C144" s="7" t="s">
         <v>14</v>
@@ -3677,67 +3680,67 @@
     </row>
     <row r="145" spans="2:4" s="6" customFormat="1">
       <c r="B145" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="C145" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D145" s="4"/>
+    </row>
+    <row r="146" spans="2:4" s="6" customFormat="1">
+      <c r="B146" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="C145" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D145" s="4"/>
-    </row>
-    <row r="146" spans="2:4" s="6" customFormat="1">
-      <c r="B146" s="22"/>
-      <c r="C146" s="7"/>
+      <c r="C146" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="D146" s="4"/>
     </row>
     <row r="147" spans="2:4" s="6" customFormat="1">
-      <c r="B147" s="20" t="s">
+      <c r="B147" s="22"/>
+      <c r="C147" s="7"/>
+      <c r="D147" s="4"/>
+    </row>
+    <row r="148" spans="2:4" s="6" customFormat="1">
+      <c r="B148" s="20" t="s">
         <v>122</v>
       </c>
-      <c r="C147" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D147" s="4"/>
-    </row>
-    <row r="148" spans="2:4" s="6" customFormat="1">
-      <c r="B148" s="22"/>
-      <c r="C148" s="7"/>
+      <c r="C148" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="D148" s="4"/>
     </row>
     <row r="149" spans="2:4" s="6" customFormat="1">
-      <c r="B149" s="20" t="s">
+      <c r="B149" s="22"/>
+      <c r="C149" s="7"/>
+      <c r="D149" s="4"/>
+    </row>
+    <row r="150" spans="2:4" s="6" customFormat="1">
+      <c r="B150" s="20" t="s">
         <v>123</v>
       </c>
-      <c r="C149" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D149" s="4"/>
-    </row>
-    <row r="150" spans="2:4" s="6" customFormat="1">
-      <c r="B150" s="23" t="s">
+      <c r="C150" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D150" s="4"/>
+    </row>
+    <row r="151" spans="2:4" s="6" customFormat="1">
+      <c r="B151" s="23" t="s">
         <v>124</v>
       </c>
-      <c r="C150" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D150" s="4"/>
-    </row>
-    <row r="151" spans="2:4" s="6" customFormat="1">
-      <c r="B151" s="20"/>
-      <c r="C151" s="7"/>
+      <c r="C151" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="D151" s="4"/>
     </row>
     <row r="152" spans="2:4" s="6" customFormat="1">
-      <c r="B152" s="20" t="s">
+      <c r="B152" s="20"/>
+      <c r="C152" s="7"/>
+      <c r="D152" s="4"/>
+    </row>
+    <row r="153" spans="2:4" s="6" customFormat="1">
+      <c r="B153" s="20" t="s">
         <v>125</v>
-      </c>
-      <c r="C152" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D152" s="4"/>
-    </row>
-    <row r="153" spans="2:4" s="6" customFormat="1">
-      <c r="B153" s="23" t="s">
-        <v>126</v>
       </c>
       <c r="C153" s="7" t="s">
         <v>14</v>
@@ -3746,30 +3749,30 @@
     </row>
     <row r="154" spans="2:4" s="6" customFormat="1">
       <c r="B154" s="23" t="s">
+        <v>126</v>
+      </c>
+      <c r="C154" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D154" s="4"/>
+    </row>
+    <row r="155" spans="2:4" s="6" customFormat="1">
+      <c r="B155" s="23" t="s">
         <v>127</v>
       </c>
-      <c r="C154" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D154" s="4"/>
-    </row>
-    <row r="155" spans="2:4" s="6" customFormat="1">
-      <c r="B155" s="22"/>
-      <c r="C155" s="7"/>
+      <c r="C155" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="D155" s="4"/>
     </row>
     <row r="156" spans="2:4" s="6" customFormat="1">
-      <c r="B156" s="20" t="s">
+      <c r="B156" s="22"/>
+      <c r="C156" s="7"/>
+      <c r="D156" s="4"/>
+    </row>
+    <row r="157" spans="2:4" s="6" customFormat="1">
+      <c r="B157" s="20" t="s">
         <v>129</v>
-      </c>
-      <c r="C156" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D156" s="4"/>
-    </row>
-    <row r="157" spans="2:4" s="6" customFormat="1">
-      <c r="B157" s="23" t="s">
-        <v>52</v>
       </c>
       <c r="C157" s="7" t="s">
         <v>14</v>
@@ -3778,30 +3781,30 @@
     </row>
     <row r="158" spans="2:4" s="6" customFormat="1">
       <c r="B158" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="C158" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D158" s="4"/>
+    </row>
+    <row r="159" spans="2:4" s="6" customFormat="1">
+      <c r="B159" s="23" t="s">
         <v>130</v>
       </c>
-      <c r="C158" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D158" s="4"/>
-    </row>
-    <row r="159" spans="2:4" s="6" customFormat="1">
-      <c r="B159" s="20"/>
-      <c r="C159" s="7"/>
+      <c r="C159" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="D159" s="4"/>
     </row>
     <row r="160" spans="2:4" s="6" customFormat="1">
-      <c r="B160" s="20" t="s">
+      <c r="B160" s="20"/>
+      <c r="C160" s="7"/>
+      <c r="D160" s="4"/>
+    </row>
+    <row r="161" spans="2:4" s="6" customFormat="1">
+      <c r="B161" s="20" t="s">
         <v>131</v>
-      </c>
-      <c r="C160" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D160" s="4"/>
-    </row>
-    <row r="161" spans="2:4" s="6" customFormat="1">
-      <c r="B161" s="23" t="s">
-        <v>52</v>
       </c>
       <c r="C161" s="7" t="s">
         <v>14</v>
@@ -3810,30 +3813,30 @@
     </row>
     <row r="162" spans="2:4" s="6" customFormat="1">
       <c r="B162" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="C162" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D162" s="4"/>
+    </row>
+    <row r="163" spans="2:4" s="6" customFormat="1">
+      <c r="B163" s="23" t="s">
         <v>130</v>
       </c>
-      <c r="C162" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D162" s="4"/>
-    </row>
-    <row r="163" spans="2:4" s="6" customFormat="1">
-      <c r="B163" s="20"/>
-      <c r="C163" s="7"/>
+      <c r="C163" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="D163" s="4"/>
     </row>
     <row r="164" spans="2:4" s="6" customFormat="1">
-      <c r="B164" s="20" t="s">
+      <c r="B164" s="20"/>
+      <c r="C164" s="7"/>
+      <c r="D164" s="4"/>
+    </row>
+    <row r="165" spans="2:4" s="6" customFormat="1">
+      <c r="B165" s="20" t="s">
         <v>132</v>
-      </c>
-      <c r="C164" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D164" s="4"/>
-    </row>
-    <row r="165" spans="2:4" s="6" customFormat="1">
-      <c r="B165" s="23" t="s">
-        <v>133</v>
       </c>
       <c r="C165" s="7" t="s">
         <v>14</v>
@@ -3842,51 +3845,51 @@
     </row>
     <row r="166" spans="2:4" s="6" customFormat="1">
       <c r="B166" s="23" t="s">
+        <v>133</v>
+      </c>
+      <c r="C166" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D166" s="4"/>
+    </row>
+    <row r="167" spans="2:4" s="6" customFormat="1">
+      <c r="B167" s="23" t="s">
         <v>127</v>
       </c>
-      <c r="C166" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D166" s="4"/>
-    </row>
-    <row r="167" spans="2:4" s="6" customFormat="1">
-      <c r="B167" s="23"/>
-      <c r="C167" s="7"/>
+      <c r="C167" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="D167" s="4"/>
     </row>
     <row r="168" spans="2:4" s="6" customFormat="1">
-      <c r="B168" s="20" t="s">
+      <c r="B168" s="23"/>
+      <c r="C168" s="7"/>
+      <c r="D168" s="4"/>
+    </row>
+    <row r="169" spans="2:4" s="6" customFormat="1">
+      <c r="B169" s="20" t="s">
         <v>128</v>
       </c>
-      <c r="C168" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D168" s="4"/>
-    </row>
-    <row r="169" spans="2:4" s="6" customFormat="1">
-      <c r="B169" s="20"/>
-      <c r="C169" s="7"/>
+      <c r="C169" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="D169" s="4"/>
     </row>
     <row r="170" spans="2:4" s="6" customFormat="1">
-      <c r="B170" s="27" t="s">
-        <v>54</v>
-      </c>
+      <c r="B170" s="20"/>
       <c r="C170" s="7"/>
       <c r="D170" s="4"/>
     </row>
     <row r="171" spans="2:4" s="6" customFormat="1">
-      <c r="B171" s="20" t="s">
+      <c r="B171" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="C171" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="C171" s="7"/>
       <c r="D171" s="4"/>
     </row>
     <row r="172" spans="2:4" s="6" customFormat="1">
-      <c r="B172" s="23" t="s">
-        <v>214</v>
+      <c r="B172" s="20" t="s">
+        <v>54</v>
       </c>
       <c r="C172" s="7" t="s">
         <v>14</v>
@@ -3895,94 +3898,98 @@
     </row>
     <row r="173" spans="2:4" s="6" customFormat="1">
       <c r="B173" s="23" t="s">
+        <v>214</v>
+      </c>
+      <c r="C173" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D173" s="4"/>
+    </row>
+    <row r="174" spans="2:4" s="6" customFormat="1">
+      <c r="B174" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="C173" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D173" s="4"/>
-    </row>
-    <row r="174" spans="2:4" s="6" customFormat="1">
-      <c r="B174" s="20" t="s">
+      <c r="C174" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D174" s="4"/>
+    </row>
+    <row r="175" spans="2:4" s="6" customFormat="1">
+      <c r="B175" s="20" t="s">
         <v>216</v>
       </c>
-      <c r="C174" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D174" s="4"/>
-    </row>
-    <row r="175" spans="2:4" s="6" customFormat="1">
-      <c r="B175" s="22"/>
-      <c r="C175" s="7"/>
+      <c r="C175" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="D175" s="4"/>
     </row>
     <row r="176" spans="2:4" s="6" customFormat="1">
-      <c r="B176" s="20" t="s">
+      <c r="B176" s="22"/>
+      <c r="C176" s="7"/>
+      <c r="D176" s="4"/>
+    </row>
+    <row r="177" spans="2:4" s="6" customFormat="1">
+      <c r="B177" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="C176" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D176" s="4"/>
-    </row>
-    <row r="177" spans="2:4" s="6" customFormat="1">
-      <c r="B177" s="23" t="s">
+      <c r="C177" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D177" s="4"/>
+    </row>
+    <row r="178" spans="2:4" s="6" customFormat="1">
+      <c r="B178" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="C177" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D177" s="4"/>
-    </row>
-    <row r="178" spans="2:4" s="6" customFormat="1">
-      <c r="B178" s="22"/>
-      <c r="C178" s="7"/>
+      <c r="C178" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="D178" s="4"/>
     </row>
     <row r="179" spans="2:4" s="6" customFormat="1">
-      <c r="B179" s="20" t="s">
+      <c r="B179" s="22"/>
+      <c r="C179" s="7"/>
+      <c r="D179" s="4"/>
+    </row>
+    <row r="180" spans="2:4" s="6" customFormat="1">
+      <c r="B180" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="C179" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D179" s="4"/>
-    </row>
-    <row r="180" spans="2:4" s="6" customFormat="1">
-      <c r="B180" s="23" t="s">
+      <c r="C180" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D180" s="4"/>
+    </row>
+    <row r="181" spans="2:4" s="6" customFormat="1">
+      <c r="B181" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="C180" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D180" s="4"/>
-    </row>
-    <row r="181" spans="2:4" s="6" customFormat="1">
-      <c r="B181" s="22"/>
-      <c r="C181" s="7"/>
+      <c r="C181" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="D181" s="4"/>
     </row>
     <row r="182" spans="2:4" s="6" customFormat="1">
-      <c r="B182" s="20" t="s">
+      <c r="B182" s="22"/>
+      <c r="C182" s="7"/>
+      <c r="D182" s="4"/>
+    </row>
+    <row r="183" spans="2:4" s="6" customFormat="1">
+      <c r="B183" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="C182" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D182" s="4"/>
-    </row>
-    <row r="183" spans="2:4" s="6" customFormat="1">
-      <c r="B183" s="23" t="s">
+      <c r="C183" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D183" s="4"/>
+    </row>
+    <row r="184" spans="2:4" s="6" customFormat="1">
+      <c r="B184" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="C183" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D183" s="4"/>
-    </row>
-    <row r="184" spans="2:4" s="6" customFormat="1">
-      <c r="B184" s="20"/>
-      <c r="C184" s="7"/>
+      <c r="C184" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="D184" s="4"/>
     </row>
     <row r="185" spans="2:4" s="6" customFormat="1">
@@ -3991,17 +3998,13 @@
       <c r="D185" s="4"/>
     </row>
     <row r="186" spans="2:4" s="6" customFormat="1">
-      <c r="B186" s="27" t="s">
+      <c r="B186" s="20"/>
+      <c r="C186" s="7"/>
+      <c r="D186" s="4"/>
+    </row>
+    <row r="187" spans="2:4" s="6" customFormat="1">
+      <c r="B187" s="27" t="s">
         <v>134</v>
-      </c>
-      <c r="C186" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D186" s="4"/>
-    </row>
-    <row r="187" spans="2:4" s="6" customFormat="1">
-      <c r="B187" s="20" t="s">
-        <v>163</v>
       </c>
       <c r="C187" s="7" t="s">
         <v>2</v>
@@ -4010,7 +4013,7 @@
     </row>
     <row r="188" spans="2:4" s="6" customFormat="1">
       <c r="B188" s="20" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C188" s="7" t="s">
         <v>2</v>
@@ -4018,8 +4021,8 @@
       <c r="D188" s="4"/>
     </row>
     <row r="189" spans="2:4" s="6" customFormat="1">
-      <c r="B189" s="22" t="s">
-        <v>165</v>
+      <c r="B189" s="20" t="s">
+        <v>164</v>
       </c>
       <c r="C189" s="7" t="s">
         <v>2</v>
@@ -4027,8 +4030,8 @@
       <c r="D189" s="4"/>
     </row>
     <row r="190" spans="2:4" s="6" customFormat="1">
-      <c r="B190" s="20" t="s">
-        <v>85</v>
+      <c r="B190" s="22" t="s">
+        <v>165</v>
       </c>
       <c r="C190" s="7" t="s">
         <v>2</v>
@@ -4037,7 +4040,7 @@
     </row>
     <row r="191" spans="2:4" s="6" customFormat="1">
       <c r="B191" s="20" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C191" s="7" t="s">
         <v>2</v>
@@ -4045,55 +4048,56 @@
       <c r="D191" s="4"/>
     </row>
     <row r="192" spans="2:4" s="6" customFormat="1">
-      <c r="B192" s="22"/>
-      <c r="C192" s="7"/>
+      <c r="B192" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="C192" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="D192" s="4"/>
     </row>
     <row r="193" spans="2:4" s="6" customFormat="1">
-      <c r="B193" s="20"/>
+      <c r="B193" s="22"/>
       <c r="C193" s="7"/>
       <c r="D193" s="4"/>
     </row>
     <row r="194" spans="2:4" s="6" customFormat="1">
-      <c r="B194" s="19"/>
+      <c r="B194" s="20"/>
       <c r="C194" s="7"/>
       <c r="D194" s="4"/>
     </row>
     <row r="195" spans="2:4" s="6" customFormat="1">
-      <c r="B195" s="4"/>
+      <c r="B195" s="19"/>
       <c r="C195" s="7"/>
       <c r="D195" s="4"/>
     </row>
     <row r="196" spans="2:4" s="6" customFormat="1">
-      <c r="B196" s="3" t="s">
-        <v>24</v>
-      </c>
+      <c r="B196" s="4"/>
       <c r="C196" s="7"/>
       <c r="D196" s="4"/>
     </row>
-    <row r="197" spans="2:4">
+    <row r="197" spans="2:4" s="6" customFormat="1">
+      <c r="B197" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="C197" s="7"/>
+      <c r="D197" s="4"/>
     </row>
     <row r="198" spans="2:4">
-      <c r="B198" s="43" t="s">
+      <c r="C198" s="7"/>
+    </row>
+    <row r="199" spans="2:4">
+      <c r="B199" s="43" t="s">
         <v>137</v>
       </c>
-      <c r="C198" s="7"/>
-    </row>
-    <row r="199" spans="2:4">
       <c r="C199" s="7"/>
     </row>
     <row r="200" spans="2:4">
-      <c r="B200" t="s">
-        <v>81</v>
-      </c>
-      <c r="C200" s="9" t="s">
-        <v>14</v>
-      </c>
+      <c r="C200" s="7"/>
     </row>
     <row r="201" spans="2:4">
       <c r="B201" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C201" s="9" t="s">
         <v>14</v>
@@ -4101,7 +4105,7 @@
     </row>
     <row r="202" spans="2:4">
       <c r="B202" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C202" s="9" t="s">
         <v>14</v>
@@ -4109,7 +4113,7 @@
     </row>
     <row r="203" spans="2:4">
       <c r="B203" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C203" s="9" t="s">
         <v>14</v>
@@ -4117,15 +4121,15 @@
     </row>
     <row r="204" spans="2:4">
       <c r="B204" t="s">
-        <v>85</v>
-      </c>
-      <c r="C204" s="7" t="s">
-        <v>2</v>
+        <v>84</v>
+      </c>
+      <c r="C204" s="9" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="205" spans="2:4">
       <c r="B205" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C205" s="7" t="s">
         <v>2</v>
@@ -4133,55 +4137,55 @@
     </row>
     <row r="206" spans="2:4">
       <c r="B206" t="s">
+        <v>86</v>
+      </c>
+      <c r="C206" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="207" spans="2:4">
+      <c r="B207" t="s">
         <v>87</v>
       </c>
-      <c r="C206" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="207" spans="2:4">
-      <c r="B207" s="44" t="s">
+      <c r="C207" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="208" spans="2:4">
+      <c r="B208" s="44" t="s">
         <v>89</v>
       </c>
-      <c r="C207" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="208" spans="2:4">
-      <c r="B208" t="s">
+      <c r="C208" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="209" spans="2:3">
+      <c r="B209" t="s">
         <v>88</v>
       </c>
-      <c r="C208" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="209" spans="2:3">
-      <c r="B209" s="44" t="s">
+      <c r="C209" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="210" spans="2:3">
+      <c r="B210" s="44" t="s">
         <v>90</v>
       </c>
-      <c r="C209" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="210" spans="2:3">
-      <c r="B210" t="s">
+      <c r="C210" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="211" spans="2:3">
+      <c r="B211" t="s">
         <v>92</v>
       </c>
-      <c r="C210" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="211" spans="2:3">
-      <c r="B211" s="44" t="s">
+      <c r="C211" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="212" spans="2:3">
+      <c r="B212" s="44" t="s">
         <v>93</v>
-      </c>
-      <c r="C211" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="212" spans="2:3">
-      <c r="B212" s="45" t="s">
-        <v>103</v>
       </c>
       <c r="C212" s="9" t="s">
         <v>14</v>
@@ -4189,15 +4193,19 @@
     </row>
     <row r="213" spans="2:3">
       <c r="B213" s="45" t="s">
+        <v>103</v>
+      </c>
+      <c r="C213" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="214" spans="2:3">
+      <c r="B214" s="45" t="s">
         <v>117</v>
       </c>
-      <c r="C213" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="214" spans="2:3">
-      <c r="B214" s="44"/>
-      <c r="C214" s="9"/>
+      <c r="C214" s="9" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="215" spans="2:3">
       <c r="B215" s="44"/>
@@ -4208,6 +4216,7 @@
       <c r="C216" s="9"/>
     </row>
     <row r="217" spans="2:3">
+      <c r="B217" s="44"/>
       <c r="C217" s="9"/>
     </row>
     <row r="218" spans="2:3">
@@ -4220,25 +4229,20 @@
       <c r="C220" s="9"/>
     </row>
     <row r="221" spans="2:3">
-      <c r="B221" s="43" t="s">
+      <c r="C221" s="9"/>
+    </row>
+    <row r="222" spans="2:3">
+      <c r="B222" s="43" t="s">
         <v>138</v>
       </c>
-      <c r="C221" s="9"/>
-    </row>
-    <row r="222" spans="2:3">
       <c r="C222" s="9"/>
     </row>
     <row r="223" spans="2:3">
-      <c r="B223" t="s">
-        <v>111</v>
-      </c>
-      <c r="C223" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="C223" s="9"/>
     </row>
     <row r="224" spans="2:3">
       <c r="B224" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C224" s="7" t="s">
         <v>14</v>
@@ -4246,7 +4250,7 @@
     </row>
     <row r="225" spans="2:3">
       <c r="B225" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C225" s="7" t="s">
         <v>14</v>
@@ -4254,7 +4258,7 @@
     </row>
     <row r="226" spans="2:3">
       <c r="B226" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C226" s="7" t="s">
         <v>14</v>
@@ -4262,7 +4266,7 @@
     </row>
     <row r="227" spans="2:3">
       <c r="B227" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C227" s="7" t="s">
         <v>14</v>
@@ -4270,7 +4274,7 @@
     </row>
     <row r="228" spans="2:3">
       <c r="B228" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C228" s="7" t="s">
         <v>14</v>
@@ -4278,14 +4282,19 @@
     </row>
     <row r="229" spans="2:3">
       <c r="B229" t="s">
+        <v>116</v>
+      </c>
+      <c r="C229" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="230" spans="2:3">
+      <c r="B230" t="s">
         <v>148</v>
       </c>
-      <c r="C229" s="7" t="s">
+      <c r="C230" s="7" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="230" spans="2:3">
-      <c r="C230" s="9"/>
     </row>
     <row r="231" spans="2:3">
       <c r="C231" s="9"/>
@@ -4294,97 +4303,97 @@
       <c r="C232" s="9"/>
     </row>
     <row r="233" spans="2:3">
-      <c r="B233" s="43" t="s">
+      <c r="C233" s="9"/>
+    </row>
+    <row r="234" spans="2:3">
+      <c r="B234" s="43" t="s">
         <v>139</v>
       </c>
-      <c r="C233" s="9"/>
-    </row>
-    <row r="234" spans="2:3">
       <c r="C234" s="9"/>
     </row>
     <row r="235" spans="2:3">
-      <c r="B235" t="s">
-        <v>135</v>
-      </c>
-      <c r="C235" s="9" t="s">
-        <v>14</v>
-      </c>
+      <c r="C235" s="9"/>
     </row>
     <row r="236" spans="2:3">
       <c r="B236" t="s">
+        <v>135</v>
+      </c>
+      <c r="C236" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="237" spans="2:3">
+      <c r="B237" t="s">
         <v>102</v>
       </c>
-      <c r="C236" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="238" spans="2:3">
-      <c r="B238" t="s">
-        <v>80</v>
-      </c>
-      <c r="C238" s="9" t="s">
+      <c r="C237" s="9" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="239" spans="2:3">
       <c r="B239" t="s">
-        <v>94</v>
-      </c>
-      <c r="C239" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C239" s="9" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="240" spans="2:3">
       <c r="B240" t="s">
+        <v>94</v>
+      </c>
+      <c r="C240" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="241" spans="2:3">
+      <c r="B241" t="s">
         <v>95</v>
       </c>
-      <c r="C240" s="7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="241" spans="2:3">
-      <c r="C241" s="9"/>
+      <c r="C241" s="7" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="242" spans="2:3">
-      <c r="B242" s="45" t="s">
+      <c r="C242" s="9"/>
+    </row>
+    <row r="243" spans="2:3">
+      <c r="B243" s="45" t="s">
         <v>101</v>
       </c>
-      <c r="C242" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="243" spans="2:3">
-      <c r="C243" s="9"/>
+      <c r="C243" s="9" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="244" spans="2:3">
-      <c r="B244" s="45" t="s">
+      <c r="C244" s="9"/>
+    </row>
+    <row r="245" spans="2:3">
+      <c r="B245" s="45" t="s">
         <v>99</v>
       </c>
-      <c r="C244" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="245" spans="2:3">
-      <c r="B245" t="s">
+      <c r="C245" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="246" spans="2:3">
+      <c r="B246" t="s">
         <v>100</v>
       </c>
-      <c r="C245" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="246" spans="2:3">
-      <c r="C246" s="9"/>
+      <c r="C246" s="9" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="247" spans="2:3">
-      <c r="B247" t="s">
+      <c r="C247" s="9"/>
+    </row>
+    <row r="248" spans="2:3">
+      <c r="B248" t="s">
         <v>187</v>
       </c>
-      <c r="C247" s="7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="248" spans="2:3">
-      <c r="C248" s="9"/>
+      <c r="C248" s="7" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="249" spans="2:3">
       <c r="C249" s="9"/>
@@ -4402,67 +4411,67 @@
       <c r="C253" s="9"/>
     </row>
     <row r="254" spans="2:3">
-      <c r="B254" s="3" t="s">
+      <c r="C254" s="9"/>
+    </row>
+    <row r="255" spans="2:3">
+      <c r="B255" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C254" s="9"/>
-    </row>
-    <row r="255" spans="2:3">
-      <c r="B255" t="s">
-        <v>49</v>
-      </c>
-      <c r="C255" s="7" t="s">
-        <v>2</v>
-      </c>
+      <c r="C255" s="9"/>
     </row>
     <row r="256" spans="2:3">
       <c r="B256" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C256" s="7" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
     </row>
     <row r="257" spans="2:4">
       <c r="B257" t="s">
+        <v>50</v>
+      </c>
+      <c r="C257" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="258" spans="2:4">
+      <c r="B258" t="s">
         <v>51</v>
       </c>
-      <c r="C257" s="7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="258" spans="2:4">
-      <c r="C258" s="9"/>
+      <c r="C258" s="7" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="259" spans="2:4">
-      <c r="B259" t="s">
-        <v>97</v>
-      </c>
-      <c r="C259" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="C259" s="9"/>
     </row>
     <row r="260" spans="2:4">
       <c r="B260" t="s">
+        <v>97</v>
+      </c>
+      <c r="C260" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="261" spans="2:4">
+      <c r="B261" t="s">
         <v>98</v>
       </c>
-      <c r="C260" s="7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="261" spans="2:4">
-      <c r="C261" s="9"/>
+      <c r="C261" s="7" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="262" spans="2:4">
-      <c r="B262" t="s">
+      <c r="C262" s="9"/>
+    </row>
+    <row r="263" spans="2:4">
+      <c r="B263" t="s">
         <v>148</v>
       </c>
-      <c r="C262" s="7" t="s">
+      <c r="C263" s="7" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="263" spans="2:4">
-      <c r="C263" s="9"/>
     </row>
     <row r="264" spans="2:4">
       <c r="C264" s="9"/>
@@ -4473,30 +4482,24 @@
     <row r="266" spans="2:4">
       <c r="C266" s="9"/>
     </row>
-    <row r="268" spans="2:4" s="6" customFormat="1">
-      <c r="B268" s="3" t="s">
+    <row r="267" spans="2:4">
+      <c r="C267" s="9"/>
+    </row>
+    <row r="269" spans="2:4" s="6" customFormat="1">
+      <c r="B269" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C268" s="7"/>
-      <c r="D268" s="4"/>
-    </row>
-    <row r="269" spans="2:4" s="6" customFormat="1">
-      <c r="B269" s="22"/>
       <c r="C269" s="7"/>
       <c r="D269" s="4"/>
     </row>
     <row r="270" spans="2:4" s="6" customFormat="1">
-      <c r="B270" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="C270" s="7" t="s">
-        <v>2</v>
-      </c>
+      <c r="B270" s="22"/>
+      <c r="C270" s="7"/>
       <c r="D270" s="4"/>
     </row>
     <row r="271" spans="2:4" s="6" customFormat="1">
       <c r="B271" s="22" t="s">
-        <v>193</v>
+        <v>49</v>
       </c>
       <c r="C271" s="7" t="s">
         <v>2</v>
@@ -4505,133 +4508,133 @@
     </row>
     <row r="272" spans="2:4" s="6" customFormat="1">
       <c r="B272" s="22" t="s">
-        <v>50</v>
+        <v>193</v>
       </c>
       <c r="C272" s="7" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="D272" s="4"/>
     </row>
     <row r="273" spans="2:4" s="6" customFormat="1">
       <c r="B273" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="C273" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D273" s="4"/>
+    </row>
+    <row r="274" spans="2:4" s="6" customFormat="1">
+      <c r="B274" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="C273" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D273" s="4"/>
-    </row>
-    <row r="274" spans="2:4" s="6" customFormat="1">
-      <c r="B274" s="22"/>
-      <c r="C274" s="7"/>
+      <c r="C274" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="D274" s="4"/>
     </row>
     <row r="275" spans="2:4" s="6" customFormat="1">
-      <c r="B275" s="22" t="s">
-        <v>97</v>
-      </c>
-      <c r="C275" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="B275" s="22"/>
+      <c r="C275" s="7"/>
       <c r="D275" s="4"/>
     </row>
     <row r="276" spans="2:4" s="6" customFormat="1">
       <c r="B276" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="C276" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D276" s="4"/>
+    </row>
+    <row r="277" spans="2:4" s="6" customFormat="1">
+      <c r="B277" s="22" t="s">
         <v>98</v>
       </c>
-      <c r="C276" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D276" s="4"/>
-    </row>
-    <row r="277" spans="2:4" s="6" customFormat="1">
-      <c r="B277" s="22"/>
-      <c r="C277" s="7"/>
+      <c r="C277" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="D277" s="4"/>
     </row>
     <row r="278" spans="2:4" s="6" customFormat="1">
-      <c r="B278" t="s">
+      <c r="B278" s="22"/>
+      <c r="C278" s="7"/>
+      <c r="D278" s="4"/>
+    </row>
+    <row r="279" spans="2:4" s="6" customFormat="1">
+      <c r="B279" t="s">
         <v>148</v>
       </c>
-      <c r="C278" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D278" s="4"/>
-    </row>
-    <row r="279" spans="2:4" s="6" customFormat="1">
-      <c r="B279" s="22"/>
-      <c r="C279" s="7"/>
+      <c r="C279" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="D279" s="4"/>
     </row>
     <row r="280" spans="2:4" s="6" customFormat="1">
-      <c r="B280" s="22" t="s">
-        <v>174</v>
-      </c>
-      <c r="C280" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="B280" s="22"/>
+      <c r="C280" s="7"/>
       <c r="D280" s="4"/>
     </row>
     <row r="281" spans="2:4" s="6" customFormat="1">
       <c r="B281" s="22" t="s">
+        <v>174</v>
+      </c>
+      <c r="C281" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D281" s="4"/>
+    </row>
+    <row r="282" spans="2:4" s="6" customFormat="1">
+      <c r="B282" s="22" t="s">
         <v>175</v>
       </c>
-      <c r="C281" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D281" s="4"/>
-    </row>
-    <row r="282" spans="2:4" s="6" customFormat="1">
-      <c r="C282" s="7"/>
+      <c r="C282" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="D282" s="4"/>
     </row>
     <row r="283" spans="2:4" s="6" customFormat="1">
-      <c r="B283" s="9" t="s">
+      <c r="C283" s="7"/>
+      <c r="D283" s="4"/>
+    </row>
+    <row r="284" spans="2:4" s="6" customFormat="1">
+      <c r="B284" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="C283" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D283" s="4"/>
-    </row>
-    <row r="284" spans="2:4" s="6" customFormat="1">
-      <c r="B284" s="22"/>
-      <c r="C284" s="7"/>
+      <c r="C284" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="D284" s="4"/>
     </row>
     <row r="285" spans="2:4" s="6" customFormat="1">
-      <c r="B285" s="22" t="s">
+      <c r="B285" s="22"/>
+      <c r="C285" s="7"/>
+      <c r="D285" s="4"/>
+    </row>
+    <row r="286" spans="2:4" s="6" customFormat="1">
+      <c r="B286" s="22" t="s">
         <v>186</v>
       </c>
-      <c r="C285" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D285" s="4"/>
-    </row>
-    <row r="286" spans="2:4" s="6" customFormat="1">
-      <c r="B286" s="22"/>
-      <c r="C286" s="7"/>
+      <c r="C286" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="D286" s="4"/>
     </row>
     <row r="287" spans="2:4" s="6" customFormat="1">
-      <c r="B287" s="22" t="s">
-        <v>178</v>
-      </c>
+      <c r="B287" s="22"/>
       <c r="C287" s="7"/>
       <c r="D287" s="4"/>
     </row>
     <row r="288" spans="2:4" s="6" customFormat="1">
-      <c r="B288" s="20" t="s">
-        <v>172</v>
-      </c>
-      <c r="C288" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="B288" s="22" t="s">
+        <v>178</v>
+      </c>
+      <c r="C288" s="7"/>
       <c r="D288" s="4"/>
     </row>
     <row r="289" spans="2:4" s="6" customFormat="1">
       <c r="B289" s="20" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C289" s="7" t="s">
         <v>14</v>
@@ -4640,7 +4643,7 @@
     </row>
     <row r="290" spans="2:4" s="6" customFormat="1">
       <c r="B290" s="20" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C290" s="7" t="s">
         <v>14</v>
@@ -4649,7 +4652,7 @@
     </row>
     <row r="291" spans="2:4" s="6" customFormat="1">
       <c r="B291" s="20" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C291" s="7" t="s">
         <v>14</v>
@@ -4658,53 +4661,57 @@
     </row>
     <row r="292" spans="2:4" s="6" customFormat="1">
       <c r="B292" s="20" t="s">
+        <v>177</v>
+      </c>
+      <c r="C292" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D292" s="4"/>
+    </row>
+    <row r="293" spans="2:4" s="6" customFormat="1">
+      <c r="B293" s="20" t="s">
         <v>180</v>
       </c>
-      <c r="C292" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D292" s="4"/>
-    </row>
-    <row r="293" spans="2:4" s="6" customFormat="1">
-      <c r="B293" s="22"/>
-      <c r="C293" s="7"/>
+      <c r="C293" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="D293" s="4"/>
     </row>
     <row r="294" spans="2:4" s="6" customFormat="1">
-      <c r="B294" s="22" t="s">
-        <v>184</v>
-      </c>
-      <c r="C294" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="B294" s="22"/>
+      <c r="C294" s="7"/>
       <c r="D294" s="4"/>
     </row>
     <row r="295" spans="2:4" s="6" customFormat="1">
       <c r="B295" s="22" t="s">
+        <v>184</v>
+      </c>
+      <c r="C295" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D295" s="4"/>
+    </row>
+    <row r="296" spans="2:4" s="6" customFormat="1">
+      <c r="B296" s="22" t="s">
         <v>185</v>
       </c>
-      <c r="C295" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D295" s="4"/>
-    </row>
-    <row r="296" spans="2:4" s="6" customFormat="1">
-      <c r="B296" s="22"/>
-      <c r="C296" s="7"/>
+      <c r="C296" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="D296" s="4"/>
     </row>
     <row r="297" spans="2:4" s="6" customFormat="1">
-      <c r="B297" s="22" t="s">
+      <c r="B297" s="22"/>
+      <c r="C297" s="7"/>
+      <c r="D297" s="4"/>
+    </row>
+    <row r="298" spans="2:4" s="6" customFormat="1">
+      <c r="B298" s="22" t="s">
         <v>99</v>
       </c>
-      <c r="C297" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D297" s="4"/>
-    </row>
-    <row r="298" spans="2:4" s="6" customFormat="1">
-      <c r="B298" s="22"/>
-      <c r="C298" s="7"/>
+      <c r="C298" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="D298" s="4"/>
     </row>
     <row r="299" spans="2:4" s="6" customFormat="1">
@@ -4723,38 +4730,34 @@
       <c r="D301" s="4"/>
     </row>
     <row r="302" spans="2:4" s="6" customFormat="1">
-      <c r="B302" s="3" t="s">
-        <v>21</v>
-      </c>
+      <c r="B302" s="22"/>
       <c r="C302" s="7"/>
       <c r="D302" s="4"/>
     </row>
     <row r="303" spans="2:4" s="6" customFormat="1">
-      <c r="B303" s="22"/>
+      <c r="B303" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="C303" s="7"/>
       <c r="D303" s="4"/>
     </row>
     <row r="304" spans="2:4" s="6" customFormat="1">
-      <c r="B304" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="C304" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="B304" s="22"/>
+      <c r="C304" s="7"/>
       <c r="D304" s="4"/>
     </row>
     <row r="305" spans="2:4" s="6" customFormat="1">
       <c r="B305" s="22" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C305" s="7" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="D305" s="4"/>
     </row>
     <row r="306" spans="2:4" s="6" customFormat="1">
       <c r="B306" s="22" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C306" s="7" t="s">
         <v>2</v>
@@ -4763,53 +4766,53 @@
     </row>
     <row r="307" spans="2:4" s="6" customFormat="1">
       <c r="B307" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="C307" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D307" s="4"/>
+    </row>
+    <row r="308" spans="2:4" s="6" customFormat="1">
+      <c r="B308" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="C307" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D307" s="4"/>
-    </row>
-    <row r="308" spans="2:4" s="6" customFormat="1">
-      <c r="B308" s="22"/>
-      <c r="C308" s="7"/>
+      <c r="C308" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="D308" s="4"/>
     </row>
     <row r="309" spans="2:4" s="6" customFormat="1">
-      <c r="B309" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="C309" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="B309" s="22"/>
+      <c r="C309" s="7"/>
       <c r="D309" s="4"/>
     </row>
     <row r="310" spans="2:4" s="6" customFormat="1">
       <c r="B310" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="C310" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D310" s="4"/>
+    </row>
+    <row r="311" spans="2:4" s="6" customFormat="1">
+      <c r="B311" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="C310" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D310" s="4"/>
-    </row>
-    <row r="311" spans="2:4" s="6" customFormat="1">
-      <c r="B311" s="22"/>
-      <c r="C311" s="7"/>
+      <c r="C311" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="D311" s="4"/>
     </row>
     <row r="312" spans="2:4" s="6" customFormat="1">
-      <c r="B312" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="C312" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="B312" s="22"/>
+      <c r="C312" s="7"/>
       <c r="D312" s="4"/>
     </row>
     <row r="313" spans="2:4" s="6" customFormat="1">
       <c r="B313" s="22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C313" s="7" t="s">
         <v>14</v>
@@ -4818,44 +4821,48 @@
     </row>
     <row r="314" spans="2:4" s="6" customFormat="1">
       <c r="B314" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="C314" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D314" s="4"/>
+    </row>
+    <row r="315" spans="2:4" s="6" customFormat="1">
+      <c r="B315" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="C314" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D314" s="4"/>
-    </row>
-    <row r="315" spans="2:4" s="6" customFormat="1">
-      <c r="B315" s="22"/>
-      <c r="C315" s="7"/>
+      <c r="C315" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="D315" s="4"/>
     </row>
     <row r="316" spans="2:4" s="6" customFormat="1">
-      <c r="B316" s="22" t="s">
+      <c r="B316" s="22"/>
+      <c r="C316" s="7"/>
+      <c r="D316" s="4"/>
+    </row>
+    <row r="317" spans="2:4" s="6" customFormat="1">
+      <c r="B317" s="22" t="s">
         <v>140</v>
       </c>
-      <c r="C316" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D316" s="4"/>
-    </row>
-    <row r="317" spans="2:4" s="6" customFormat="1">
-      <c r="B317" s="22"/>
-      <c r="C317" s="7"/>
+      <c r="C317" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="D317" s="4"/>
     </row>
     <row r="318" spans="2:4" s="6" customFormat="1">
-      <c r="B318" s="22" t="s">
+      <c r="B318" s="22"/>
+      <c r="C318" s="7"/>
+      <c r="D318" s="4"/>
+    </row>
+    <row r="319" spans="2:4" s="6" customFormat="1">
+      <c r="B319" s="22" t="s">
         <v>194</v>
       </c>
-      <c r="C318" s="7" t="s">
+      <c r="C319" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D318" s="4"/>
-    </row>
-    <row r="319" spans="2:4" s="6" customFormat="1">
-      <c r="B319" s="22"/>
-      <c r="C319" s="7"/>
       <c r="D319" s="4"/>
     </row>
     <row r="320" spans="2:4" s="6" customFormat="1">
@@ -4879,36 +4886,32 @@
       <c r="D323" s="4"/>
     </row>
     <row r="324" spans="2:4" s="6" customFormat="1">
-      <c r="B324" s="3" t="s">
-        <v>152</v>
-      </c>
+      <c r="B324" s="22"/>
       <c r="C324" s="7"/>
       <c r="D324" s="4"/>
     </row>
     <row r="325" spans="2:4" s="6" customFormat="1">
-      <c r="B325" s="22"/>
+      <c r="B325" s="3" t="s">
+        <v>152</v>
+      </c>
       <c r="C325" s="7"/>
       <c r="D325" s="4"/>
     </row>
     <row r="326" spans="2:4" s="6" customFormat="1">
-      <c r="B326" s="22" t="s">
-        <v>153</v>
-      </c>
+      <c r="B326" s="22"/>
       <c r="C326" s="7"/>
       <c r="D326" s="4"/>
     </row>
     <row r="327" spans="2:4" s="6" customFormat="1">
-      <c r="B327" s="20" t="s">
-        <v>158</v>
-      </c>
-      <c r="C327" s="7" t="s">
-        <v>2</v>
-      </c>
+      <c r="B327" s="22" t="s">
+        <v>153</v>
+      </c>
+      <c r="C327" s="7"/>
       <c r="D327" s="4"/>
     </row>
     <row r="328" spans="2:4" s="6" customFormat="1">
       <c r="B328" s="20" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="C328" s="7" t="s">
         <v>2</v>
@@ -4917,46 +4920,46 @@
     </row>
     <row r="329" spans="2:4" s="6" customFormat="1">
       <c r="B329" s="20" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C329" s="7" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="D329" s="4"/>
     </row>
     <row r="330" spans="2:4" s="6" customFormat="1">
       <c r="B330" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="C330" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D330" s="4"/>
+    </row>
+    <row r="331" spans="2:4" s="6" customFormat="1">
+      <c r="B331" s="20" t="s">
         <v>161</v>
       </c>
-      <c r="C330" s="7" t="s">
+      <c r="C331" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D330" s="4"/>
-    </row>
-    <row r="331" spans="2:4" s="6" customFormat="1">
-      <c r="B331" s="22"/>
-      <c r="C331" s="7"/>
       <c r="D331" s="4"/>
     </row>
     <row r="332" spans="2:4" s="6" customFormat="1">
-      <c r="B332" s="22" t="s">
-        <v>33</v>
-      </c>
+      <c r="B332" s="22"/>
       <c r="C332" s="7"/>
       <c r="D332" s="4"/>
     </row>
     <row r="333" spans="2:4" s="6" customFormat="1">
-      <c r="B333" s="20" t="s">
-        <v>155</v>
-      </c>
-      <c r="C333" s="7" t="s">
-        <v>2</v>
-      </c>
+      <c r="B333" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="C333" s="7"/>
       <c r="D333" s="4"/>
     </row>
     <row r="334" spans="2:4" s="6" customFormat="1">
       <c r="B334" s="20" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C334" s="7" t="s">
         <v>2</v>
@@ -4964,45 +4967,49 @@
       <c r="D334" s="4"/>
     </row>
     <row r="335" spans="2:4" s="6" customFormat="1">
-      <c r="B335" s="22"/>
-      <c r="C335" s="7"/>
+      <c r="B335" s="20" t="s">
+        <v>156</v>
+      </c>
+      <c r="C335" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="D335" s="4"/>
     </row>
     <row r="336" spans="2:4" s="6" customFormat="1">
-      <c r="B336" s="22" t="s">
-        <v>170</v>
-      </c>
-      <c r="C336" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="B336" s="22"/>
+      <c r="C336" s="7"/>
       <c r="D336" s="4"/>
     </row>
     <row r="337" spans="2:4" s="6" customFormat="1">
       <c r="B337" s="22" t="s">
+        <v>170</v>
+      </c>
+      <c r="C337" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D337" s="4"/>
+    </row>
+    <row r="338" spans="2:4" s="6" customFormat="1">
+      <c r="B338" s="22" t="s">
         <v>171</v>
       </c>
-      <c r="C337" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D337" s="4"/>
-    </row>
-    <row r="338" spans="2:4" s="6" customFormat="1">
-      <c r="B338" s="22"/>
-      <c r="C338" s="7"/>
+      <c r="C338" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="D338" s="4"/>
     </row>
     <row r="339" spans="2:4" s="6" customFormat="1">
-      <c r="B339" s="22" t="s">
+      <c r="B339" s="22"/>
+      <c r="C339" s="7"/>
+      <c r="D339" s="4"/>
+    </row>
+    <row r="340" spans="2:4" s="6" customFormat="1">
+      <c r="B340" s="22" t="s">
         <v>203</v>
       </c>
-      <c r="C339" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D339" s="4"/>
-    </row>
-    <row r="340" spans="2:4" s="6" customFormat="1">
-      <c r="B340" s="22"/>
-      <c r="C340" s="7"/>
+      <c r="C340" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="D340" s="4"/>
     </row>
     <row r="341" spans="2:4" s="6" customFormat="1">
@@ -5021,17 +5028,13 @@
       <c r="D343" s="4"/>
     </row>
     <row r="344" spans="2:4" s="6" customFormat="1">
-      <c r="B344" s="22" t="s">
+      <c r="B344" s="22"/>
+      <c r="C344" s="7"/>
+      <c r="D344" s="4"/>
+    </row>
+    <row r="345" spans="2:4" s="6" customFormat="1">
+      <c r="B345" s="22" t="s">
         <v>204</v>
-      </c>
-      <c r="C344" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D344" s="4"/>
-    </row>
-    <row r="345" spans="2:4" s="6" customFormat="1">
-      <c r="B345" s="20" t="s">
-        <v>206</v>
       </c>
       <c r="C345" s="7" t="s">
         <v>14</v>
@@ -5040,7 +5043,7 @@
     </row>
     <row r="346" spans="2:4" s="6" customFormat="1">
       <c r="B346" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C346" s="7" t="s">
         <v>14</v>
@@ -5049,34 +5052,38 @@
     </row>
     <row r="347" spans="2:4" s="6" customFormat="1">
       <c r="B347" s="20" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C347" s="7" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="D347" s="4"/>
     </row>
     <row r="348" spans="2:4" s="6" customFormat="1">
       <c r="B348" s="20" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C348" s="7" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="D348" s="4"/>
     </row>
     <row r="349" spans="2:4" s="6" customFormat="1">
       <c r="B349" s="20" t="s">
+        <v>209</v>
+      </c>
+      <c r="C349" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D349" s="4"/>
+    </row>
+    <row r="350" spans="2:4" s="6" customFormat="1">
+      <c r="B350" s="20" t="s">
         <v>210</v>
       </c>
-      <c r="C349" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D349" s="4"/>
-    </row>
-    <row r="350" spans="2:4" s="6" customFormat="1">
-      <c r="B350" s="22"/>
-      <c r="C350" s="7"/>
+      <c r="C350" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="D350" s="4"/>
     </row>
     <row r="351" spans="2:4" s="6" customFormat="1">
@@ -5141,16 +5148,16 @@
     </row>
     <row r="363" spans="1:4" s="6" customFormat="1">
       <c r="B363" s="22"/>
-      <c r="C363" s="4"/>
+      <c r="C363" s="7"/>
       <c r="D363" s="4"/>
     </row>
     <row r="364" spans="1:4" s="6" customFormat="1">
-      <c r="B364" s="19"/>
+      <c r="B364" s="22"/>
       <c r="C364" s="4"/>
       <c r="D364" s="4"/>
     </row>
     <row r="365" spans="1:4" s="6" customFormat="1">
-      <c r="B365" s="21"/>
+      <c r="B365" s="19"/>
       <c r="C365" s="4"/>
       <c r="D365" s="4"/>
     </row>
@@ -5159,76 +5166,81 @@
       <c r="C366" s="4"/>
       <c r="D366" s="4"/>
     </row>
-    <row r="367" spans="1:4">
-      <c r="A367" s="3"/>
-      <c r="B367" s="11"/>
-      <c r="C367" s="11"/>
-      <c r="D367" s="3"/>
+    <row r="367" spans="1:4" s="6" customFormat="1">
+      <c r="B367" s="21"/>
+      <c r="C367" s="4"/>
+      <c r="D367" s="4"/>
     </row>
     <row r="368" spans="1:4">
       <c r="A368" s="3"/>
-      <c r="B368" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C368" s="6">
-        <f>COUNTIF(C5:C367,"y")</f>
-        <v>48</v>
-      </c>
-      <c r="D368" s="2"/>
+      <c r="B368" s="11"/>
+      <c r="C368" s="11"/>
+      <c r="D368" s="3"/>
     </row>
     <row r="369" spans="1:4">
       <c r="A369" s="3"/>
       <c r="B369" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C369" s="6">
-        <f>COUNTIF(C5:C367,"n")</f>
-        <v>159</v>
+        <f>COUNTIF(C5:C368,"y")</f>
+        <v>50</v>
       </c>
       <c r="D369" s="2"/>
     </row>
     <row r="370" spans="1:4">
       <c r="A370" s="3"/>
       <c r="B370" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C370" s="7">
-        <f>COUNTIF(C5:C367,"TBD")</f>
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C370" s="6">
+        <f>COUNTIF(C5:C368,"n")</f>
+        <v>158</v>
       </c>
       <c r="D370" s="2"/>
     </row>
     <row r="371" spans="1:4">
       <c r="A371" s="3"/>
       <c r="B371" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C371" s="7">
+        <f>COUNTIF(C5:C368,"TBD")</f>
+        <v>0</v>
+      </c>
+      <c r="D371" s="2"/>
+    </row>
+    <row r="372" spans="1:4">
+      <c r="A372" s="3"/>
+      <c r="B372" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C371">
-        <f>SUM(C368:C370)</f>
-        <v>207</v>
-      </c>
-      <c r="D371" s="2"/>
-    </row>
-    <row r="372" spans="1:4" ht="18">
-      <c r="A372" s="3"/>
-      <c r="B372" s="10"/>
-      <c r="C372" s="10" t="s">
+      <c r="C372">
+        <f>SUM(C369:C371)</f>
+        <v>208</v>
+      </c>
+      <c r="D372" s="2"/>
+    </row>
+    <row r="373" spans="1:4" ht="18">
+      <c r="A373" s="3"/>
+      <c r="B373" s="10"/>
+      <c r="C373" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D372" s="41">
-        <f>C368/(C369+C368 + C370)</f>
-        <v>0.2318840579710145</v>
-      </c>
-    </row>
-    <row r="373" spans="1:4">
-      <c r="A373" s="3"/>
-      <c r="B373" s="11"/>
-      <c r="C373" s="11"/>
-      <c r="D373" s="3"/>
+      <c r="D373" s="41">
+        <f>C369/(C370+C369 + C371)</f>
+        <v>0.24038461538461539</v>
+      </c>
+    </row>
+    <row r="374" spans="1:4">
+      <c r="A374" s="3"/>
+      <c r="B374" s="11"/>
+      <c r="C374" s="11"/>
+      <c r="D374" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
-  <conditionalFormatting sqref="C268:C65121 C238:C266 C1:C3 C6:C236">
+  <conditionalFormatting sqref="C269:C65122 C239:C267 C1:C3 C6:C237">
     <cfRule type="cellIs" dxfId="2" priority="10" stopIfTrue="1" operator="equal">
       <formula>"y"</formula>
     </cfRule>
@@ -5254,7 +5266,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="10020" topLeftCell="A46" activePane="bottomLeft"/>
-      <selection pane="bottomLeft" activeCell="F55" sqref="F55"/>
+      <selection pane="bottomLeft" activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.5"/>
@@ -5656,10 +5668,10 @@
         <v>42911</v>
       </c>
       <c r="B55" s="4">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C55" s="4">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D55" s="4">
         <v>0</v>
@@ -5670,7 +5682,7 @@
       <c r="F55" s="48"/>
       <c r="G55" s="30">
         <f t="shared" ref="G55" si="3">B55/SUM(B55:E55)</f>
-        <v>0.23076923076923078</v>
+        <v>0.23923444976076555</v>
       </c>
       <c r="H55" s="7"/>
     </row>
@@ -5715,25 +5727,25 @@
       </c>
       <c r="G58" s="38">
         <f>MIN(G55)</f>
-        <v>0.23076923076923078</v>
+        <v>0.23923444976076555</v>
       </c>
       <c r="H58" s="7"/>
     </row>
     <row r="59" spans="1:11">
       <c r="A59" s="39">
         <f>SUM(B59:D59)</f>
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B59" s="15">
-        <f>Features!C368</f>
-        <v>48</v>
+        <f>Features!C369</f>
+        <v>50</v>
       </c>
       <c r="C59" s="16">
-        <f>Features!C369</f>
-        <v>159</v>
+        <f>Features!C370</f>
+        <v>158</v>
       </c>
       <c r="D59" s="17">
-        <f>Features!C370</f>
+        <f>Features!C371</f>
         <v>0</v>
       </c>
       <c r="E59" s="18">
@@ -5781,7 +5793,7 @@
       </c>
       <c r="B63" s="49">
         <f>(A55-A48)*A59/B59 +A48</f>
-        <v>43613.25</v>
+        <v>43580.92</v>
       </c>
       <c r="C63" s="4"/>
       <c r="D63" s="7"/>

</xml_diff>

<commit_message>
select word on double click
</commit_message>
<xml_diff>
--- a/FxEditor Feature Matrix.xlsx
+++ b/FxEditor Feature Matrix.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="226">
   <si>
     <t>Feature</t>
   </si>
@@ -687,6 +687,15 @@
   </si>
   <si>
     <t>goes faster if moved further from the boundary</t>
+  </si>
+  <si>
+    <t>select line</t>
+  </si>
+  <si>
+    <t>select word at marker</t>
+  </si>
+  <si>
+    <t>pluggable word selector</t>
   </si>
 </sst>
 </file>
@@ -946,7 +955,7 @@
           <c:yMode val="edge"/>
           <c:x val="3.8461559098965002E-2"/>
           <c:y val="2.2690437601296611E-2"/>
-          <c:w val="0.91978071330955213"/>
+          <c:w val="0.91978071330955224"/>
           <c:h val="0.89627228525119951"/>
         </c:manualLayout>
       </c:layout>
@@ -979,10 +988,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Progress!$A$48:$A$58</c:f>
+              <c:f>Progress!$A$48:$A$59</c:f>
               <c:numCache>
                 <c:formatCode>yyyy\/mm\/dd</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>42699</c:v>
                 </c:pt>
@@ -1015,16 +1024,19 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>42952</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>42966</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Progress!$B$48:$B$58</c:f>
+              <c:f>Progress!$B$48:$B$59</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1057,6 +1069,9 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>90</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1089,10 +1104,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Progress!$A$48:$A$58</c:f>
+              <c:f>Progress!$A$48:$A$59</c:f>
               <c:numCache>
                 <c:formatCode>yyyy\/mm\/dd</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>42699</c:v>
                 </c:pt>
@@ -1125,16 +1140,19 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>42952</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>42966</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Progress!$C$48:$C$58</c:f>
+              <c:f>Progress!$C$48:$C$59</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1167,6 +1185,9 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>131</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>129</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1199,10 +1220,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Progress!$A$48:$A$58</c:f>
+              <c:f>Progress!$A$48:$A$59</c:f>
               <c:numCache>
                 <c:formatCode>yyyy\/mm\/dd</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>42699</c:v>
                 </c:pt>
@@ -1235,16 +1256,19 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>42952</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>42966</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Progress!$D$48:$D$58</c:f>
+              <c:f>Progress!$D$48:$D$59</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1276,6 +1300,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1309,10 +1336,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Progress!$A$48:$A$58</c:f>
+              <c:f>Progress!$A$48:$A$59</c:f>
               <c:numCache>
                 <c:formatCode>yyyy\/mm\/dd</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>42699</c:v>
                 </c:pt>
@@ -1345,16 +1372,19 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>42952</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>42966</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Progress!$E$48:$E$62</c:f>
+              <c:f>Progress!$E$48:$E$63</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1388,21 +1418,24 @@
                 <c:pt idx="10">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="11">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="145272192"/>
-        <c:axId val="145101952"/>
+        <c:axId val="126266752"/>
+        <c:axId val="126030976"/>
       </c:areaChart>
       <c:dateAx>
-        <c:axId val="145272192"/>
+        <c:axId val="126266752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1435,7 +1468,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="145101952"/>
+        <c:crossAx val="126030976"/>
         <c:crosses val="autoZero"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
@@ -1445,7 +1478,7 @@
         <c:minorTimeUnit val="months"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="145101952"/>
+        <c:axId val="126030976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1487,7 +1520,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="145272192"/>
+        <c:crossAx val="126266752"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1510,7 +1543,7 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="4.5828229804607823E-2"/>
-          <c:y val="0.33819556996218403"/>
+          <c:y val="0.33819556996218414"/>
           <c:w val="0.12857154394162268"/>
           <c:h val="0.11669367909238262"/>
         </c:manualLayout>
@@ -1577,7 +1610,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="1" l="0.75000000000001388" r="0.75000000000001388" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75000000000001399" r="0.75000000000001399" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup paperSize="9" orientation="landscape" horizontalDpi="1200" verticalDpi="1200"/>
   </c:printSettings>
 </c:chartSpace>
@@ -1631,7 +1664,7 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="4.4510450248127581E-2"/>
+          <c:x val="4.4510450248127595E-2"/>
           <c:y val="0.10032394165889739"/>
           <c:w val="0.79228601441663349"/>
           <c:h val="0.79935527708863363"/>
@@ -1666,10 +1699,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Progress!$A$48:$A$58</c:f>
+              <c:f>Progress!$A$48:$A$59</c:f>
               <c:numCache>
                 <c:formatCode>yyyy\/mm\/dd</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>42699</c:v>
                 </c:pt>
@@ -1702,16 +1735,19 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>42952</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>42966</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Progress!$G$48:$G$58</c:f>
+              <c:f>Progress!$G$48:$G$59</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1744,16 +1780,19 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0.39069767441860465</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.41095890410958902</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="145125760"/>
-        <c:axId val="145127296"/>
+        <c:axId val="126054784"/>
+        <c:axId val="126056320"/>
       </c:areaChart>
       <c:dateAx>
-        <c:axId val="145125760"/>
+        <c:axId val="126054784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1761,13 +1800,13 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="yyyy\/mm\/dd" sourceLinked="1"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="145127296"/>
+        <c:crossAx val="126056320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="145127296"/>
+        <c:axId val="126056320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1810,7 +1849,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="145125760"/>
+        <c:crossAx val="126054784"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1859,7 +1898,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="1" l="0.75000000000001388" r="0.75000000000001388" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75000000000001399" r="0.75000000000001399" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
   </c:printSettings>
 </c:chartSpace>
@@ -1910,10 +1949,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Progress!$A$48:$A$58</c:f>
+              <c:f>Progress!$A$48:$A$59</c:f>
               <c:numCache>
                 <c:formatCode>yyyy\/mm\/dd</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>42699</c:v>
                 </c:pt>
@@ -1946,16 +1985,19 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>42952</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>42966</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Progress!$C$48:$C$58</c:f>
+              <c:f>Progress!$C$48:$C$59</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1988,6 +2030,9 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>131</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>129</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2020,10 +2065,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Progress!$A$48:$A$58</c:f>
+              <c:f>Progress!$A$48:$A$59</c:f>
               <c:numCache>
                 <c:formatCode>yyyy\/mm\/dd</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>42699</c:v>
                 </c:pt>
@@ -2056,16 +2101,19 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>42952</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>42966</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Progress!$D$48:$D$58</c:f>
+              <c:f>Progress!$D$48:$D$59</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -2097,17 +2145,20 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="145152256"/>
-        <c:axId val="145158144"/>
+        <c:axId val="126081280"/>
+        <c:axId val="126615552"/>
       </c:areaChart>
       <c:dateAx>
-        <c:axId val="145152256"/>
+        <c:axId val="126081280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2140,7 +2191,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="145158144"/>
+        <c:crossAx val="126615552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
@@ -2149,7 +2200,7 @@
         <c:minorTimeUnit val="months"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="145158144"/>
+        <c:axId val="126615552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2191,7 +2242,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="145152256"/>
+        <c:crossAx val="126081280"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2240,7 +2291,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="1" l="0.75000000000001388" r="0.75000000000001388" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75000000000001399" r="0.75000000000001399" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
   </c:printSettings>
 </c:chartSpace>
@@ -2290,7 +2341,7 @@
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>65</xdr:row>
+      <xdr:row>66</xdr:row>
       <xdr:rowOff>123826</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2698,10 +2749,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D387"/>
+  <dimension ref="A1:D391"/>
   <sheetViews>
-    <sheetView topLeftCell="A127" workbookViewId="0">
-      <selection activeCell="C192" sqref="C192"/>
+    <sheetView topLeftCell="A304" workbookViewId="0">
+      <selection activeCell="B350" sqref="B350"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.5"/>
@@ -3683,7 +3734,7 @@
         <v>165</v>
       </c>
       <c r="C128" s="7" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="D128" s="4"/>
     </row>
@@ -3692,7 +3743,7 @@
         <v>166</v>
       </c>
       <c r="C129" s="7" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="D129" s="4"/>
     </row>
@@ -5200,60 +5251,72 @@
       <c r="D346" s="4"/>
     </row>
     <row r="347" spans="2:4" s="6" customFormat="1">
-      <c r="B347" s="20"/>
-      <c r="C347" s="7"/>
+      <c r="B347" s="22" t="s">
+        <v>146</v>
+      </c>
+      <c r="C347" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="D347" s="4"/>
     </row>
     <row r="348" spans="2:4" s="6" customFormat="1">
-      <c r="B348" s="20"/>
-      <c r="C348" s="7"/>
+      <c r="B348" s="22" t="s">
+        <v>223</v>
+      </c>
+      <c r="C348" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="D348" s="4"/>
     </row>
     <row r="349" spans="2:4" s="6" customFormat="1">
-      <c r="B349" s="22"/>
-      <c r="C349" s="7"/>
+      <c r="B349" s="22" t="s">
+        <v>224</v>
+      </c>
+      <c r="C349" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="D349" s="4"/>
     </row>
     <row r="350" spans="2:4" s="6" customFormat="1">
-      <c r="B350" s="22" t="s">
-        <v>168</v>
+      <c r="B350" s="20" t="s">
+        <v>225</v>
       </c>
       <c r="C350" s="7" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="D350" s="4"/>
     </row>
     <row r="351" spans="2:4" s="6" customFormat="1">
-      <c r="B351" s="22" t="s">
-        <v>169</v>
-      </c>
-      <c r="C351" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="B351" s="22"/>
+      <c r="C351" s="7"/>
       <c r="D351" s="4"/>
     </row>
     <row r="352" spans="2:4" s="6" customFormat="1">
-      <c r="B352" s="22"/>
+      <c r="B352" s="20"/>
       <c r="C352" s="7"/>
       <c r="D352" s="4"/>
     </row>
     <row r="353" spans="2:4" s="6" customFormat="1">
-      <c r="B353" s="22" t="s">
-        <v>201</v>
-      </c>
-      <c r="C353" s="7" t="s">
+      <c r="B353" s="22"/>
+      <c r="C353" s="7"/>
+      <c r="D353" s="4"/>
+    </row>
+    <row r="354" spans="2:4" s="6" customFormat="1">
+      <c r="B354" s="22" t="s">
+        <v>168</v>
+      </c>
+      <c r="C354" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D353" s="4"/>
-    </row>
-    <row r="354" spans="2:4" s="6" customFormat="1">
-      <c r="B354" s="22"/>
-      <c r="C354" s="7"/>
       <c r="D354" s="4"/>
     </row>
     <row r="355" spans="2:4" s="6" customFormat="1">
-      <c r="B355" s="22"/>
-      <c r="C355" s="7"/>
+      <c r="B355" s="22" t="s">
+        <v>169</v>
+      </c>
+      <c r="C355" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="D355" s="4"/>
     </row>
     <row r="356" spans="2:4" s="6" customFormat="1">
@@ -5262,49 +5325,37 @@
       <c r="D356" s="4"/>
     </row>
     <row r="357" spans="2:4" s="6" customFormat="1">
-      <c r="B357" s="22"/>
-      <c r="C357" s="7"/>
+      <c r="B357" s="22" t="s">
+        <v>201</v>
+      </c>
+      <c r="C357" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="D357" s="4"/>
     </row>
     <row r="358" spans="2:4" s="6" customFormat="1">
-      <c r="B358" s="22" t="s">
+      <c r="B358" s="22"/>
+      <c r="C358" s="7"/>
+      <c r="D358" s="4"/>
+    </row>
+    <row r="359" spans="2:4" s="6" customFormat="1">
+      <c r="B359" s="22"/>
+      <c r="C359" s="7"/>
+      <c r="D359" s="4"/>
+    </row>
+    <row r="360" spans="2:4" s="6" customFormat="1">
+      <c r="B360" s="22"/>
+      <c r="C360" s="7"/>
+      <c r="D360" s="4"/>
+    </row>
+    <row r="361" spans="2:4" s="6" customFormat="1">
+      <c r="B361" s="22"/>
+      <c r="C361" s="7"/>
+      <c r="D361" s="4"/>
+    </row>
+    <row r="362" spans="2:4" s="6" customFormat="1">
+      <c r="B362" s="22" t="s">
         <v>202</v>
-      </c>
-      <c r="C358" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D358" s="4"/>
-    </row>
-    <row r="359" spans="2:4" s="6" customFormat="1">
-      <c r="B359" s="20" t="s">
-        <v>204</v>
-      </c>
-      <c r="C359" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D359" s="4"/>
-    </row>
-    <row r="360" spans="2:4" s="6" customFormat="1">
-      <c r="B360" s="20" t="s">
-        <v>205</v>
-      </c>
-      <c r="C360" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D360" s="4"/>
-    </row>
-    <row r="361" spans="2:4" s="6" customFormat="1">
-      <c r="B361" s="20" t="s">
-        <v>206</v>
-      </c>
-      <c r="C361" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D361" s="4"/>
-    </row>
-    <row r="362" spans="2:4" s="6" customFormat="1">
-      <c r="B362" s="20" t="s">
-        <v>207</v>
       </c>
       <c r="C362" s="7" t="s">
         <v>14</v>
@@ -5313,7 +5364,7 @@
     </row>
     <row r="363" spans="2:4" s="6" customFormat="1">
       <c r="B363" s="20" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="C363" s="7" t="s">
         <v>14</v>
@@ -5321,23 +5372,39 @@
       <c r="D363" s="4"/>
     </row>
     <row r="364" spans="2:4" s="6" customFormat="1">
-      <c r="B364" s="22"/>
-      <c r="C364" s="7"/>
+      <c r="B364" s="20" t="s">
+        <v>205</v>
+      </c>
+      <c r="C364" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="D364" s="4"/>
     </row>
     <row r="365" spans="2:4" s="6" customFormat="1">
-      <c r="B365" s="22"/>
-      <c r="C365" s="7"/>
+      <c r="B365" s="20" t="s">
+        <v>206</v>
+      </c>
+      <c r="C365" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="D365" s="4"/>
     </row>
     <row r="366" spans="2:4" s="6" customFormat="1">
-      <c r="B366" s="22"/>
-      <c r="C366" s="7"/>
+      <c r="B366" s="20" t="s">
+        <v>207</v>
+      </c>
+      <c r="C366" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="D366" s="4"/>
     </row>
     <row r="367" spans="2:4" s="6" customFormat="1">
-      <c r="B367" s="22"/>
-      <c r="C367" s="7"/>
+      <c r="B367" s="20" t="s">
+        <v>208</v>
+      </c>
+      <c r="C367" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="D367" s="4"/>
     </row>
     <row r="368" spans="2:4" s="6" customFormat="1">
@@ -5345,136 +5412,156 @@
       <c r="C368" s="7"/>
       <c r="D368" s="4"/>
     </row>
-    <row r="369" spans="1:4" s="6" customFormat="1">
+    <row r="369" spans="2:4" s="6" customFormat="1">
       <c r="B369" s="22"/>
       <c r="C369" s="7"/>
       <c r="D369" s="4"/>
     </row>
-    <row r="370" spans="1:4" s="6" customFormat="1">
+    <row r="370" spans="2:4" s="6" customFormat="1">
       <c r="B370" s="22"/>
       <c r="C370" s="7"/>
       <c r="D370" s="4"/>
     </row>
-    <row r="371" spans="1:4" s="6" customFormat="1">
+    <row r="371" spans="2:4" s="6" customFormat="1">
       <c r="B371" s="22"/>
       <c r="C371" s="7"/>
       <c r="D371" s="4"/>
     </row>
-    <row r="372" spans="1:4" s="6" customFormat="1">
+    <row r="372" spans="2:4" s="6" customFormat="1">
       <c r="B372" s="22"/>
       <c r="C372" s="7"/>
       <c r="D372" s="4"/>
     </row>
-    <row r="373" spans="1:4" s="6" customFormat="1">
+    <row r="373" spans="2:4" s="6" customFormat="1">
       <c r="B373" s="22"/>
       <c r="C373" s="7"/>
       <c r="D373" s="4"/>
     </row>
-    <row r="374" spans="1:4" s="6" customFormat="1">
+    <row r="374" spans="2:4" s="6" customFormat="1">
       <c r="B374" s="22"/>
       <c r="C374" s="7"/>
       <c r="D374" s="4"/>
     </row>
-    <row r="375" spans="1:4" s="6" customFormat="1">
+    <row r="375" spans="2:4" s="6" customFormat="1">
       <c r="B375" s="22"/>
       <c r="C375" s="7"/>
       <c r="D375" s="4"/>
     </row>
-    <row r="376" spans="1:4" s="6" customFormat="1">
+    <row r="376" spans="2:4" s="6" customFormat="1">
       <c r="B376" s="22"/>
       <c r="C376" s="7"/>
       <c r="D376" s="4"/>
     </row>
-    <row r="377" spans="1:4" s="6" customFormat="1">
+    <row r="377" spans="2:4" s="6" customFormat="1">
       <c r="B377" s="22"/>
-      <c r="C377" s="4"/>
+      <c r="C377" s="7"/>
       <c r="D377" s="4"/>
     </row>
-    <row r="378" spans="1:4" s="6" customFormat="1">
-      <c r="B378" s="19"/>
-      <c r="C378" s="4"/>
+    <row r="378" spans="2:4" s="6" customFormat="1">
+      <c r="B378" s="22"/>
+      <c r="C378" s="7"/>
       <c r="D378" s="4"/>
     </row>
-    <row r="379" spans="1:4" s="6" customFormat="1">
-      <c r="B379" s="21"/>
-      <c r="C379" s="4"/>
+    <row r="379" spans="2:4" s="6" customFormat="1">
+      <c r="B379" s="22"/>
+      <c r="C379" s="7"/>
       <c r="D379" s="4"/>
     </row>
-    <row r="380" spans="1:4" s="6" customFormat="1">
-      <c r="B380" s="21"/>
-      <c r="C380" s="4"/>
+    <row r="380" spans="2:4" s="6" customFormat="1">
+      <c r="B380" s="22"/>
+      <c r="C380" s="7"/>
       <c r="D380" s="4"/>
     </row>
-    <row r="381" spans="1:4">
-      <c r="A381" s="3"/>
-      <c r="B381" s="11"/>
-      <c r="C381" s="11"/>
-      <c r="D381" s="3"/>
-    </row>
-    <row r="382" spans="1:4">
-      <c r="A382" s="3"/>
-      <c r="B382" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C382" s="6">
-        <f>COUNTIF(C5:C381,"y")</f>
-        <v>84</v>
-      </c>
-      <c r="D382" s="2"/>
-    </row>
-    <row r="383" spans="1:4">
-      <c r="A383" s="3"/>
-      <c r="B383" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C383" s="6">
-        <f>COUNTIF(C5:C381,"n")</f>
-        <v>131</v>
-      </c>
-      <c r="D383" s="2"/>
-    </row>
-    <row r="384" spans="1:4">
-      <c r="A384" s="3"/>
-      <c r="B384" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C384" s="7">
-        <f>COUNTIF(C5:C381,"TBD")</f>
-        <v>0</v>
-      </c>
-      <c r="D384" s="2"/>
+    <row r="381" spans="2:4" s="6" customFormat="1">
+      <c r="B381" s="22"/>
+      <c r="C381" s="4"/>
+      <c r="D381" s="4"/>
+    </row>
+    <row r="382" spans="2:4" s="6" customFormat="1">
+      <c r="B382" s="19"/>
+      <c r="C382" s="4"/>
+      <c r="D382" s="4"/>
+    </row>
+    <row r="383" spans="2:4" s="6" customFormat="1">
+      <c r="B383" s="21"/>
+      <c r="C383" s="4"/>
+      <c r="D383" s="4"/>
+    </row>
+    <row r="384" spans="2:4" s="6" customFormat="1">
+      <c r="B384" s="21"/>
+      <c r="C384" s="4"/>
+      <c r="D384" s="4"/>
     </row>
     <row r="385" spans="1:4">
       <c r="A385" s="3"/>
-      <c r="B385" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C385">
-        <f>SUM(C382:C384)</f>
-        <v>215</v>
-      </c>
-      <c r="D385" s="2"/>
-    </row>
-    <row r="386" spans="1:4" ht="18">
+      <c r="B385" s="11"/>
+      <c r="C385" s="11"/>
+      <c r="D385" s="3"/>
+    </row>
+    <row r="386" spans="1:4">
       <c r="A386" s="3"/>
-      <c r="B386" s="10"/>
-      <c r="C386" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D386" s="41">
-        <f>C382/(C383+C382 + C384)</f>
-        <v>0.39069767441860465</v>
-      </c>
+      <c r="B386" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C386" s="6">
+        <f>COUNTIF(C5:C385,"y")</f>
+        <v>90</v>
+      </c>
+      <c r="D386" s="2"/>
     </row>
     <row r="387" spans="1:4">
       <c r="A387" s="3"/>
-      <c r="B387" s="11"/>
-      <c r="C387" s="11"/>
-      <c r="D387" s="3"/>
+      <c r="B387" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C387" s="6">
+        <f>COUNTIF(C5:C385,"n")</f>
+        <v>129</v>
+      </c>
+      <c r="D387" s="2"/>
+    </row>
+    <row r="388" spans="1:4">
+      <c r="A388" s="3"/>
+      <c r="B388" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C388" s="7">
+        <f>COUNTIF(C5:C385,"TBD")</f>
+        <v>0</v>
+      </c>
+      <c r="D388" s="2"/>
+    </row>
+    <row r="389" spans="1:4">
+      <c r="A389" s="3"/>
+      <c r="B389" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C389">
+        <f>SUM(C386:C388)</f>
+        <v>219</v>
+      </c>
+      <c r="D389" s="2"/>
+    </row>
+    <row r="390" spans="1:4" ht="18">
+      <c r="A390" s="3"/>
+      <c r="B390" s="10"/>
+      <c r="C390" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D390" s="41">
+        <f>C386/(C387+C386 + C388)</f>
+        <v>0.41095890410958902</v>
+      </c>
+    </row>
+    <row r="391" spans="1:4">
+      <c r="A391" s="3"/>
+      <c r="B391" s="11"/>
+      <c r="C391" s="11"/>
+      <c r="D391" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
-  <conditionalFormatting sqref="C276:C65135 C246:C274 C1:C3 C6:C244">
+  <conditionalFormatting sqref="C276:C65139 C246:C274 C1:C3 C6:C244">
     <cfRule type="cellIs" dxfId="2" priority="10" stopIfTrue="1" operator="equal">
       <formula>"y"</formula>
     </cfRule>
@@ -5496,11 +5583,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:IT872"/>
+  <dimension ref="A1:IT873"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="10020" topLeftCell="A46" activePane="bottomLeft"/>
-      <selection pane="bottomLeft" activeCell="D58" sqref="D58"/>
+      <selection pane="bottomLeft" activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.5"/>
@@ -5823,7 +5910,7 @@
       </c>
       <c r="F51" s="48"/>
       <c r="G51" s="30">
-        <f t="shared" ref="G51:G57" si="2">B51/SUM(B51:E51)</f>
+        <f t="shared" ref="G51:G58" si="2">B51/SUM(B51:E51)</f>
         <v>0.2</v>
       </c>
       <c r="H51" s="7"/>
@@ -5984,19 +6071,32 @@
       </c>
       <c r="F58" s="48"/>
       <c r="G58" s="30">
-        <f t="shared" ref="G58" si="3">B58/SUM(B58:E58)</f>
+        <f t="shared" si="2"/>
         <v>0.39069767441860465</v>
       </c>
       <c r="H58" s="7"/>
     </row>
     <row r="59" spans="1:11">
-      <c r="A59" s="47"/>
-      <c r="B59" s="4"/>
-      <c r="C59" s="4"/>
-      <c r="D59" s="4"/>
-      <c r="E59" s="4"/>
-      <c r="F59" s="28"/>
-      <c r="G59" s="30"/>
+      <c r="A59" s="47">
+        <v>42966</v>
+      </c>
+      <c r="B59" s="4">
+        <v>90</v>
+      </c>
+      <c r="C59" s="4">
+        <v>129</v>
+      </c>
+      <c r="D59" s="4">
+        <v>0</v>
+      </c>
+      <c r="E59" s="4">
+        <v>0</v>
+      </c>
+      <c r="F59" s="48"/>
+      <c r="G59" s="30">
+        <f t="shared" ref="G59" si="3">B59/SUM(B59:E59)</f>
+        <v>0.41095890410958902</v>
+      </c>
       <c r="H59" s="7"/>
     </row>
     <row r="60" spans="1:11">
@@ -6005,84 +6105,84 @@
       <c r="C60" s="4"/>
       <c r="D60" s="4"/>
       <c r="E60" s="4"/>
-      <c r="F60" s="31"/>
+      <c r="F60" s="28"/>
       <c r="G60" s="30"/>
       <c r="H60" s="7"/>
     </row>
     <row r="61" spans="1:11">
-      <c r="A61" s="14" t="s">
+      <c r="A61" s="47"/>
+      <c r="B61" s="4"/>
+      <c r="C61" s="4"/>
+      <c r="D61" s="4"/>
+      <c r="E61" s="4"/>
+      <c r="F61" s="31"/>
+      <c r="G61" s="30"/>
+      <c r="H61" s="7"/>
+    </row>
+    <row r="62" spans="1:11">
+      <c r="A62" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="B61" s="14" t="s">
+      <c r="B62" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C61" s="14" t="s">
+      <c r="C62" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="D61" s="14" t="s">
+      <c r="D62" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E61" s="14" t="s">
+      <c r="E62" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="F61" s="14" t="s">
+      <c r="F62" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="G61" s="38">
-        <f>MIN(G58)</f>
-        <v>0.39069767441860465</v>
-      </c>
-      <c r="H61" s="7"/>
-    </row>
-    <row r="62" spans="1:11">
-      <c r="A62" s="39">
-        <f>SUM(B62:D62)</f>
-        <v>215</v>
-      </c>
-      <c r="B62" s="15">
-        <f>Features!C382</f>
-        <v>84</v>
-      </c>
-      <c r="C62" s="16">
-        <f>Features!C383</f>
-        <v>131</v>
-      </c>
-      <c r="D62" s="17">
-        <f>Features!C384</f>
+      <c r="G62" s="38">
+        <f>MIN(G59)</f>
+        <v>0.41095890410958902</v>
+      </c>
+      <c r="H62" s="7"/>
+    </row>
+    <row r="63" spans="1:11">
+      <c r="A63" s="39">
+        <f>SUM(B63:D63)</f>
+        <v>219</v>
+      </c>
+      <c r="B63" s="15">
+        <f>Features!C386</f>
+        <v>90</v>
+      </c>
+      <c r="C63" s="16">
+        <f>Features!C387</f>
+        <v>129</v>
+      </c>
+      <c r="D63" s="17">
+        <f>Features!C388</f>
         <v>0</v>
       </c>
-      <c r="E62" s="18">
-        <f>MIN(E58)</f>
+      <c r="E63" s="18">
+        <f>MIN(E59)</f>
         <v>0</v>
       </c>
-      <c r="F62" s="7"/>
-      <c r="G62" s="30"/>
-      <c r="H62" s="7"/>
-    </row>
-    <row r="63" spans="1:11">
-      <c r="A63" s="4"/>
-      <c r="B63" s="19"/>
-      <c r="C63" s="4"/>
-      <c r="D63" s="7"/>
-      <c r="E63" s="7"/>
       <c r="F63" s="7"/>
       <c r="G63" s="30"/>
       <c r="H63" s="7"/>
-      <c r="J63" s="36"/>
     </row>
     <row r="64" spans="1:11">
       <c r="A64" s="4"/>
-      <c r="B64" s="4"/>
+      <c r="B64" s="19"/>
       <c r="C64" s="4"/>
       <c r="D64" s="7"/>
       <c r="E64" s="7"/>
       <c r="F64" s="7"/>
       <c r="G64" s="30"/>
       <c r="H64" s="7"/>
+      <c r="J64" s="36"/>
     </row>
     <row r="65" spans="1:8">
       <c r="A65" s="4"/>
-      <c r="B65" s="19"/>
+      <c r="B65" s="4"/>
       <c r="C65" s="4"/>
       <c r="D65" s="7"/>
       <c r="E65" s="7"/>
@@ -6091,13 +6191,8 @@
       <c r="H65" s="7"/>
     </row>
     <row r="66" spans="1:8">
-      <c r="A66" s="46" t="s">
-        <v>141</v>
-      </c>
-      <c r="B66" s="49">
-        <f>(A58-A48)*A62/B62 +A48</f>
-        <v>43346.559523809527</v>
-      </c>
+      <c r="A66" s="4"/>
+      <c r="B66" s="19"/>
       <c r="C66" s="4"/>
       <c r="D66" s="7"/>
       <c r="E66" s="7"/>
@@ -6106,8 +6201,13 @@
       <c r="H66" s="7"/>
     </row>
     <row r="67" spans="1:8">
-      <c r="A67" s="4"/>
-      <c r="B67" s="4"/>
+      <c r="A67" s="46" t="s">
+        <v>141</v>
+      </c>
+      <c r="B67" s="49">
+        <f>(A59-A48)*A63/B63 +A48</f>
+        <v>43348.7</v>
+      </c>
       <c r="C67" s="4"/>
       <c r="D67" s="7"/>
       <c r="E67" s="7"/>
@@ -6117,7 +6217,7 @@
     </row>
     <row r="68" spans="1:8">
       <c r="A68" s="4"/>
-      <c r="B68" s="19"/>
+      <c r="B68" s="4"/>
       <c r="C68" s="4"/>
       <c r="D68" s="7"/>
       <c r="E68" s="7"/>
@@ -6137,7 +6237,7 @@
     </row>
     <row r="70" spans="1:8">
       <c r="A70" s="4"/>
-      <c r="B70" s="4"/>
+      <c r="B70" s="19"/>
       <c r="C70" s="4"/>
       <c r="D70" s="7"/>
       <c r="E70" s="7"/>
@@ -6157,7 +6257,7 @@
     </row>
     <row r="72" spans="1:8">
       <c r="A72" s="4"/>
-      <c r="B72" s="7"/>
+      <c r="B72" s="4"/>
       <c r="C72" s="4"/>
       <c r="D72" s="7"/>
       <c r="E72" s="7"/>
@@ -6167,7 +6267,7 @@
     </row>
     <row r="73" spans="1:8">
       <c r="A73" s="4"/>
-      <c r="B73" s="20"/>
+      <c r="B73" s="7"/>
       <c r="C73" s="4"/>
       <c r="D73" s="7"/>
       <c r="E73" s="7"/>
@@ -6186,7 +6286,7 @@
       <c r="H74" s="7"/>
     </row>
     <row r="75" spans="1:8">
-      <c r="A75" s="7"/>
+      <c r="A75" s="4"/>
       <c r="B75" s="20"/>
       <c r="C75" s="4"/>
       <c r="D75" s="7"/>
@@ -6197,7 +6297,7 @@
     </row>
     <row r="76" spans="1:8">
       <c r="A76" s="7"/>
-      <c r="B76" s="7"/>
+      <c r="B76" s="20"/>
       <c r="C76" s="4"/>
       <c r="D76" s="7"/>
       <c r="E76" s="7"/>
@@ -6328,7 +6428,7 @@
     <row r="89" spans="1:8">
       <c r="A89" s="7"/>
       <c r="B89" s="7"/>
-      <c r="C89" s="7"/>
+      <c r="C89" s="4"/>
       <c r="D89" s="7"/>
       <c r="E89" s="7"/>
       <c r="F89" s="7"/>
@@ -6337,7 +6437,7 @@
     </row>
     <row r="90" spans="1:8">
       <c r="A90" s="7"/>
-      <c r="B90" s="6"/>
+      <c r="B90" s="7"/>
       <c r="C90" s="7"/>
       <c r="D90" s="7"/>
       <c r="E90" s="7"/>
@@ -6345,15 +6445,15 @@
       <c r="G90" s="30"/>
       <c r="H90" s="7"/>
     </row>
-    <row r="91" spans="1:8" s="2" customFormat="1">
-      <c r="A91" s="4"/>
-      <c r="B91" s="4"/>
-      <c r="C91" s="4"/>
-      <c r="D91" s="4"/>
-      <c r="E91" s="4"/>
-      <c r="F91" s="4"/>
-      <c r="G91" s="34"/>
-      <c r="H91" s="4"/>
+    <row r="91" spans="1:8">
+      <c r="A91" s="7"/>
+      <c r="B91" s="6"/>
+      <c r="C91" s="7"/>
+      <c r="D91" s="7"/>
+      <c r="E91" s="7"/>
+      <c r="F91" s="7"/>
+      <c r="G91" s="30"/>
+      <c r="H91" s="7"/>
     </row>
     <row r="92" spans="1:8" s="2" customFormat="1">
       <c r="A92" s="4"/>
@@ -6527,7 +6627,7 @@
     </row>
     <row r="109" spans="1:8" s="2" customFormat="1">
       <c r="A109" s="4"/>
-      <c r="B109" s="6"/>
+      <c r="B109" s="4"/>
       <c r="C109" s="4"/>
       <c r="D109" s="4"/>
       <c r="E109" s="4"/>
@@ -6537,7 +6637,7 @@
     </row>
     <row r="110" spans="1:8" s="2" customFormat="1">
       <c r="A110" s="4"/>
-      <c r="B110" s="4"/>
+      <c r="B110" s="6"/>
       <c r="C110" s="4"/>
       <c r="D110" s="4"/>
       <c r="E110" s="4"/>
@@ -6567,7 +6667,7 @@
     </row>
     <row r="113" spans="1:8" s="2" customFormat="1">
       <c r="A113" s="4"/>
-      <c r="B113" s="19"/>
+      <c r="B113" s="4"/>
       <c r="C113" s="4"/>
       <c r="D113" s="4"/>
       <c r="E113" s="4"/>
@@ -6607,7 +6707,7 @@
     </row>
     <row r="117" spans="1:8" s="2" customFormat="1">
       <c r="A117" s="4"/>
-      <c r="B117" s="21"/>
+      <c r="B117" s="19"/>
       <c r="C117" s="4"/>
       <c r="D117" s="4"/>
       <c r="E117" s="4"/>
@@ -6617,7 +6717,7 @@
     </row>
     <row r="118" spans="1:8" s="2" customFormat="1">
       <c r="A118" s="4"/>
-      <c r="B118" s="4"/>
+      <c r="B118" s="21"/>
       <c r="C118" s="4"/>
       <c r="D118" s="4"/>
       <c r="E118" s="4"/>
@@ -6627,7 +6727,7 @@
     </row>
     <row r="119" spans="1:8" s="2" customFormat="1">
       <c r="A119" s="4"/>
-      <c r="B119" s="6"/>
+      <c r="B119" s="4"/>
       <c r="C119" s="4"/>
       <c r="D119" s="4"/>
       <c r="E119" s="4"/>
@@ -6637,7 +6737,7 @@
     </row>
     <row r="120" spans="1:8" s="2" customFormat="1">
       <c r="A120" s="4"/>
-      <c r="B120" s="4"/>
+      <c r="B120" s="6"/>
       <c r="C120" s="4"/>
       <c r="D120" s="4"/>
       <c r="E120" s="4"/>
@@ -6647,7 +6747,7 @@
     </row>
     <row r="121" spans="1:8" s="2" customFormat="1">
       <c r="A121" s="4"/>
-      <c r="B121" s="19"/>
+      <c r="B121" s="4"/>
       <c r="C121" s="4"/>
       <c r="D121" s="4"/>
       <c r="E121" s="4"/>
@@ -6667,7 +6767,7 @@
     </row>
     <row r="123" spans="1:8" s="2" customFormat="1">
       <c r="A123" s="4"/>
-      <c r="B123" s="4"/>
+      <c r="B123" s="19"/>
       <c r="C123" s="4"/>
       <c r="D123" s="4"/>
       <c r="E123" s="4"/>
@@ -6727,7 +6827,7 @@
     </row>
     <row r="129" spans="1:8" s="2" customFormat="1">
       <c r="A129" s="4"/>
-      <c r="B129" s="19"/>
+      <c r="B129" s="4"/>
       <c r="C129" s="4"/>
       <c r="D129" s="4"/>
       <c r="E129" s="4"/>
@@ -6827,7 +6927,7 @@
     </row>
     <row r="139" spans="1:8" s="2" customFormat="1">
       <c r="A139" s="4"/>
-      <c r="B139" s="4"/>
+      <c r="B139" s="19"/>
       <c r="C139" s="4"/>
       <c r="D139" s="4"/>
       <c r="E139" s="4"/>
@@ -6877,7 +6977,7 @@
     </row>
     <row r="144" spans="1:8" s="2" customFormat="1">
       <c r="A144" s="4"/>
-      <c r="B144" s="19"/>
+      <c r="B144" s="4"/>
       <c r="C144" s="4"/>
       <c r="D144" s="4"/>
       <c r="E144" s="4"/>
@@ -6897,7 +6997,7 @@
     </row>
     <row r="146" spans="1:254" s="2" customFormat="1">
       <c r="A146" s="4"/>
-      <c r="B146" s="4"/>
+      <c r="B146" s="19"/>
       <c r="C146" s="4"/>
       <c r="D146" s="4"/>
       <c r="E146" s="4"/>
@@ -6936,284 +7036,284 @@
       <c r="H149" s="4"/>
     </row>
     <row r="150" spans="1:254" s="2" customFormat="1">
-      <c r="A150" s="21"/>
-      <c r="B150" s="21"/>
-      <c r="C150" s="21"/>
-      <c r="D150" s="21"/>
-      <c r="E150" s="21"/>
-      <c r="F150" s="21"/>
-      <c r="G150" s="35"/>
-      <c r="H150" s="21"/>
-      <c r="I150" s="5"/>
-      <c r="J150" s="5"/>
-      <c r="K150" s="5"/>
-      <c r="L150" s="5"/>
-      <c r="M150" s="5"/>
-      <c r="N150" s="5"/>
-      <c r="O150" s="5"/>
-      <c r="P150" s="5"/>
-      <c r="Q150" s="5"/>
-      <c r="R150" s="5"/>
-      <c r="S150" s="5"/>
-      <c r="T150" s="5"/>
-      <c r="U150" s="5"/>
-      <c r="V150" s="5"/>
-      <c r="W150" s="5"/>
-      <c r="X150" s="5"/>
-      <c r="Y150" s="5"/>
-      <c r="Z150" s="5"/>
-      <c r="AA150" s="5"/>
-      <c r="AB150" s="5"/>
-      <c r="AC150" s="5"/>
-      <c r="AD150" s="5"/>
-      <c r="AE150" s="5"/>
-      <c r="AF150" s="5"/>
-      <c r="AG150" s="5"/>
-      <c r="AH150" s="5"/>
-      <c r="AI150" s="5"/>
-      <c r="AJ150" s="5"/>
-      <c r="AK150" s="5"/>
-      <c r="AL150" s="5"/>
-      <c r="AM150" s="5"/>
-      <c r="AN150" s="5"/>
-      <c r="AO150" s="5"/>
-      <c r="AP150" s="5"/>
-      <c r="AQ150" s="5"/>
-      <c r="AR150" s="5"/>
-      <c r="AS150" s="5"/>
-      <c r="AT150" s="5"/>
-      <c r="AU150" s="5"/>
-      <c r="AV150" s="5"/>
-      <c r="AW150" s="5"/>
-      <c r="AX150" s="5"/>
-      <c r="AY150" s="5"/>
-      <c r="AZ150" s="5"/>
-      <c r="BA150" s="5"/>
-      <c r="BB150" s="5"/>
-      <c r="BC150" s="5"/>
-      <c r="BD150" s="5"/>
-      <c r="BE150" s="5"/>
-      <c r="BF150" s="5"/>
-      <c r="BG150" s="5"/>
-      <c r="BH150" s="5"/>
-      <c r="BI150" s="5"/>
-      <c r="BJ150" s="5"/>
-      <c r="BK150" s="5"/>
-      <c r="BL150" s="5"/>
-      <c r="BM150" s="5"/>
-      <c r="BN150" s="5"/>
-      <c r="BO150" s="5"/>
-      <c r="BP150" s="5"/>
-      <c r="BQ150" s="5"/>
-      <c r="BR150" s="5"/>
-      <c r="BS150" s="5"/>
-      <c r="BT150" s="5"/>
-      <c r="BU150" s="5"/>
-      <c r="BV150" s="5"/>
-      <c r="BW150" s="5"/>
-      <c r="BX150" s="5"/>
-      <c r="BY150" s="5"/>
-      <c r="BZ150" s="5"/>
-      <c r="CA150" s="5"/>
-      <c r="CB150" s="5"/>
-      <c r="CC150" s="5"/>
-      <c r="CD150" s="5"/>
-      <c r="CE150" s="5"/>
-      <c r="CF150" s="5"/>
-      <c r="CG150" s="5"/>
-      <c r="CH150" s="5"/>
-      <c r="CI150" s="5"/>
-      <c r="CJ150" s="5"/>
-      <c r="CK150" s="5"/>
-      <c r="CL150" s="5"/>
-      <c r="CM150" s="5"/>
-      <c r="CN150" s="5"/>
-      <c r="CO150" s="5"/>
-      <c r="CP150" s="5"/>
-      <c r="CQ150" s="5"/>
-      <c r="CR150" s="5"/>
-      <c r="CS150" s="5"/>
-      <c r="CT150" s="5"/>
-      <c r="CU150" s="5"/>
-      <c r="CV150" s="5"/>
-      <c r="CW150" s="5"/>
-      <c r="CX150" s="5"/>
-      <c r="CY150" s="5"/>
-      <c r="CZ150" s="5"/>
-      <c r="DA150" s="5"/>
-      <c r="DB150" s="5"/>
-      <c r="DC150" s="5"/>
-      <c r="DD150" s="5"/>
-      <c r="DE150" s="5"/>
-      <c r="DF150" s="5"/>
-      <c r="DG150" s="5"/>
-      <c r="DH150" s="5"/>
-      <c r="DI150" s="5"/>
-      <c r="DJ150" s="5"/>
-      <c r="DK150" s="5"/>
-      <c r="DL150" s="5"/>
-      <c r="DM150" s="5"/>
-      <c r="DN150" s="5"/>
-      <c r="DO150" s="5"/>
-      <c r="DP150" s="5"/>
-      <c r="DQ150" s="5"/>
-      <c r="DR150" s="5"/>
-      <c r="DS150" s="5"/>
-      <c r="DT150" s="5"/>
-      <c r="DU150" s="5"/>
-      <c r="DV150" s="5"/>
-      <c r="DW150" s="5"/>
-      <c r="DX150" s="5"/>
-      <c r="DY150" s="5"/>
-      <c r="DZ150" s="5"/>
-      <c r="EA150" s="5"/>
-      <c r="EB150" s="5"/>
-      <c r="EC150" s="5"/>
-      <c r="ED150" s="5"/>
-      <c r="EE150" s="5"/>
-      <c r="EF150" s="5"/>
-      <c r="EG150" s="5"/>
-      <c r="EH150" s="5"/>
-      <c r="EI150" s="5"/>
-      <c r="EJ150" s="5"/>
-      <c r="EK150" s="5"/>
-      <c r="EL150" s="5"/>
-      <c r="EM150" s="5"/>
-      <c r="EN150" s="5"/>
-      <c r="EO150" s="5"/>
-      <c r="EP150" s="5"/>
-      <c r="EQ150" s="5"/>
-      <c r="ER150" s="5"/>
-      <c r="ES150" s="5"/>
-      <c r="ET150" s="5"/>
-      <c r="EU150" s="5"/>
-      <c r="EV150" s="5"/>
-      <c r="EW150" s="5"/>
-      <c r="EX150" s="5"/>
-      <c r="EY150" s="5"/>
-      <c r="EZ150" s="5"/>
-      <c r="FA150" s="5"/>
-      <c r="FB150" s="5"/>
-      <c r="FC150" s="5"/>
-      <c r="FD150" s="5"/>
-      <c r="FE150" s="5"/>
-      <c r="FF150" s="5"/>
-      <c r="FG150" s="5"/>
-      <c r="FH150" s="5"/>
-      <c r="FI150" s="5"/>
-      <c r="FJ150" s="5"/>
-      <c r="FK150" s="5"/>
-      <c r="FL150" s="5"/>
-      <c r="FM150" s="5"/>
-      <c r="FN150" s="5"/>
-      <c r="FO150" s="5"/>
-      <c r="FP150" s="5"/>
-      <c r="FQ150" s="5"/>
-      <c r="FR150" s="5"/>
-      <c r="FS150" s="5"/>
-      <c r="FT150" s="5"/>
-      <c r="FU150" s="5"/>
-      <c r="FV150" s="5"/>
-      <c r="FW150" s="5"/>
-      <c r="FX150" s="5"/>
-      <c r="FY150" s="5"/>
-      <c r="FZ150" s="5"/>
-      <c r="GA150" s="5"/>
-      <c r="GB150" s="5"/>
-      <c r="GC150" s="5"/>
-      <c r="GD150" s="5"/>
-      <c r="GE150" s="5"/>
-      <c r="GF150" s="5"/>
-      <c r="GG150" s="5"/>
-      <c r="GH150" s="5"/>
-      <c r="GI150" s="5"/>
-      <c r="GJ150" s="5"/>
-      <c r="GK150" s="5"/>
-      <c r="GL150" s="5"/>
-      <c r="GM150" s="5"/>
-      <c r="GN150" s="5"/>
-      <c r="GO150" s="5"/>
-      <c r="GP150" s="5"/>
-      <c r="GQ150" s="5"/>
-      <c r="GR150" s="5"/>
-      <c r="GS150" s="5"/>
-      <c r="GT150" s="5"/>
-      <c r="GU150" s="5"/>
-      <c r="GV150" s="5"/>
-      <c r="GW150" s="5"/>
-      <c r="GX150" s="5"/>
-      <c r="GY150" s="5"/>
-      <c r="GZ150" s="5"/>
-      <c r="HA150" s="5"/>
-      <c r="HB150" s="5"/>
-      <c r="HC150" s="5"/>
-      <c r="HD150" s="5"/>
-      <c r="HE150" s="5"/>
-      <c r="HF150" s="5"/>
-      <c r="HG150" s="5"/>
-      <c r="HH150" s="5"/>
-      <c r="HI150" s="5"/>
-      <c r="HJ150" s="5"/>
-      <c r="HK150" s="5"/>
-      <c r="HL150" s="5"/>
-      <c r="HM150" s="5"/>
-      <c r="HN150" s="5"/>
-      <c r="HO150" s="5"/>
-      <c r="HP150" s="5"/>
-      <c r="HQ150" s="5"/>
-      <c r="HR150" s="5"/>
-      <c r="HS150" s="5"/>
-      <c r="HT150" s="5"/>
-      <c r="HU150" s="5"/>
-      <c r="HV150" s="5"/>
-      <c r="HW150" s="5"/>
-      <c r="HX150" s="5"/>
-      <c r="HY150" s="5"/>
-      <c r="HZ150" s="5"/>
-      <c r="IA150" s="5"/>
-      <c r="IB150" s="5"/>
-      <c r="IC150" s="5"/>
-      <c r="ID150" s="5"/>
-      <c r="IE150" s="5"/>
-      <c r="IF150" s="5"/>
-      <c r="IG150" s="5"/>
-      <c r="IH150" s="5"/>
-      <c r="II150" s="5"/>
-      <c r="IJ150" s="5"/>
-      <c r="IK150" s="5"/>
-      <c r="IL150" s="5"/>
-      <c r="IM150" s="5"/>
-      <c r="IN150" s="5"/>
-      <c r="IO150" s="5"/>
-      <c r="IP150" s="5"/>
-      <c r="IQ150" s="5"/>
-      <c r="IR150" s="5"/>
-      <c r="IS150" s="5"/>
-      <c r="IT150" s="5"/>
+      <c r="A150" s="4"/>
+      <c r="B150" s="4"/>
+      <c r="C150" s="4"/>
+      <c r="D150" s="4"/>
+      <c r="E150" s="4"/>
+      <c r="F150" s="4"/>
+      <c r="G150" s="34"/>
+      <c r="H150" s="4"/>
     </row>
     <row r="151" spans="1:254" s="2" customFormat="1">
-      <c r="A151" s="4"/>
-      <c r="B151" s="4"/>
-      <c r="C151" s="4"/>
-      <c r="D151" s="4"/>
-      <c r="E151" s="4"/>
-      <c r="F151" s="4"/>
-      <c r="G151" s="34"/>
-      <c r="H151" s="4"/>
-    </row>
-    <row r="152" spans="1:254">
-      <c r="A152" s="7"/>
-      <c r="B152" s="6"/>
-      <c r="C152" s="7"/>
-      <c r="D152" s="7"/>
-      <c r="E152" s="7"/>
-      <c r="F152" s="7"/>
-      <c r="G152" s="30"/>
-      <c r="H152" s="7"/>
+      <c r="A151" s="21"/>
+      <c r="B151" s="21"/>
+      <c r="C151" s="21"/>
+      <c r="D151" s="21"/>
+      <c r="E151" s="21"/>
+      <c r="F151" s="21"/>
+      <c r="G151" s="35"/>
+      <c r="H151" s="21"/>
+      <c r="I151" s="5"/>
+      <c r="J151" s="5"/>
+      <c r="K151" s="5"/>
+      <c r="L151" s="5"/>
+      <c r="M151" s="5"/>
+      <c r="N151" s="5"/>
+      <c r="O151" s="5"/>
+      <c r="P151" s="5"/>
+      <c r="Q151" s="5"/>
+      <c r="R151" s="5"/>
+      <c r="S151" s="5"/>
+      <c r="T151" s="5"/>
+      <c r="U151" s="5"/>
+      <c r="V151" s="5"/>
+      <c r="W151" s="5"/>
+      <c r="X151" s="5"/>
+      <c r="Y151" s="5"/>
+      <c r="Z151" s="5"/>
+      <c r="AA151" s="5"/>
+      <c r="AB151" s="5"/>
+      <c r="AC151" s="5"/>
+      <c r="AD151" s="5"/>
+      <c r="AE151" s="5"/>
+      <c r="AF151" s="5"/>
+      <c r="AG151" s="5"/>
+      <c r="AH151" s="5"/>
+      <c r="AI151" s="5"/>
+      <c r="AJ151" s="5"/>
+      <c r="AK151" s="5"/>
+      <c r="AL151" s="5"/>
+      <c r="AM151" s="5"/>
+      <c r="AN151" s="5"/>
+      <c r="AO151" s="5"/>
+      <c r="AP151" s="5"/>
+      <c r="AQ151" s="5"/>
+      <c r="AR151" s="5"/>
+      <c r="AS151" s="5"/>
+      <c r="AT151" s="5"/>
+      <c r="AU151" s="5"/>
+      <c r="AV151" s="5"/>
+      <c r="AW151" s="5"/>
+      <c r="AX151" s="5"/>
+      <c r="AY151" s="5"/>
+      <c r="AZ151" s="5"/>
+      <c r="BA151" s="5"/>
+      <c r="BB151" s="5"/>
+      <c r="BC151" s="5"/>
+      <c r="BD151" s="5"/>
+      <c r="BE151" s="5"/>
+      <c r="BF151" s="5"/>
+      <c r="BG151" s="5"/>
+      <c r="BH151" s="5"/>
+      <c r="BI151" s="5"/>
+      <c r="BJ151" s="5"/>
+      <c r="BK151" s="5"/>
+      <c r="BL151" s="5"/>
+      <c r="BM151" s="5"/>
+      <c r="BN151" s="5"/>
+      <c r="BO151" s="5"/>
+      <c r="BP151" s="5"/>
+      <c r="BQ151" s="5"/>
+      <c r="BR151" s="5"/>
+      <c r="BS151" s="5"/>
+      <c r="BT151" s="5"/>
+      <c r="BU151" s="5"/>
+      <c r="BV151" s="5"/>
+      <c r="BW151" s="5"/>
+      <c r="BX151" s="5"/>
+      <c r="BY151" s="5"/>
+      <c r="BZ151" s="5"/>
+      <c r="CA151" s="5"/>
+      <c r="CB151" s="5"/>
+      <c r="CC151" s="5"/>
+      <c r="CD151" s="5"/>
+      <c r="CE151" s="5"/>
+      <c r="CF151" s="5"/>
+      <c r="CG151" s="5"/>
+      <c r="CH151" s="5"/>
+      <c r="CI151" s="5"/>
+      <c r="CJ151" s="5"/>
+      <c r="CK151" s="5"/>
+      <c r="CL151" s="5"/>
+      <c r="CM151" s="5"/>
+      <c r="CN151" s="5"/>
+      <c r="CO151" s="5"/>
+      <c r="CP151" s="5"/>
+      <c r="CQ151" s="5"/>
+      <c r="CR151" s="5"/>
+      <c r="CS151" s="5"/>
+      <c r="CT151" s="5"/>
+      <c r="CU151" s="5"/>
+      <c r="CV151" s="5"/>
+      <c r="CW151" s="5"/>
+      <c r="CX151" s="5"/>
+      <c r="CY151" s="5"/>
+      <c r="CZ151" s="5"/>
+      <c r="DA151" s="5"/>
+      <c r="DB151" s="5"/>
+      <c r="DC151" s="5"/>
+      <c r="DD151" s="5"/>
+      <c r="DE151" s="5"/>
+      <c r="DF151" s="5"/>
+      <c r="DG151" s="5"/>
+      <c r="DH151" s="5"/>
+      <c r="DI151" s="5"/>
+      <c r="DJ151" s="5"/>
+      <c r="DK151" s="5"/>
+      <c r="DL151" s="5"/>
+      <c r="DM151" s="5"/>
+      <c r="DN151" s="5"/>
+      <c r="DO151" s="5"/>
+      <c r="DP151" s="5"/>
+      <c r="DQ151" s="5"/>
+      <c r="DR151" s="5"/>
+      <c r="DS151" s="5"/>
+      <c r="DT151" s="5"/>
+      <c r="DU151" s="5"/>
+      <c r="DV151" s="5"/>
+      <c r="DW151" s="5"/>
+      <c r="DX151" s="5"/>
+      <c r="DY151" s="5"/>
+      <c r="DZ151" s="5"/>
+      <c r="EA151" s="5"/>
+      <c r="EB151" s="5"/>
+      <c r="EC151" s="5"/>
+      <c r="ED151" s="5"/>
+      <c r="EE151" s="5"/>
+      <c r="EF151" s="5"/>
+      <c r="EG151" s="5"/>
+      <c r="EH151" s="5"/>
+      <c r="EI151" s="5"/>
+      <c r="EJ151" s="5"/>
+      <c r="EK151" s="5"/>
+      <c r="EL151" s="5"/>
+      <c r="EM151" s="5"/>
+      <c r="EN151" s="5"/>
+      <c r="EO151" s="5"/>
+      <c r="EP151" s="5"/>
+      <c r="EQ151" s="5"/>
+      <c r="ER151" s="5"/>
+      <c r="ES151" s="5"/>
+      <c r="ET151" s="5"/>
+      <c r="EU151" s="5"/>
+      <c r="EV151" s="5"/>
+      <c r="EW151" s="5"/>
+      <c r="EX151" s="5"/>
+      <c r="EY151" s="5"/>
+      <c r="EZ151" s="5"/>
+      <c r="FA151" s="5"/>
+      <c r="FB151" s="5"/>
+      <c r="FC151" s="5"/>
+      <c r="FD151" s="5"/>
+      <c r="FE151" s="5"/>
+      <c r="FF151" s="5"/>
+      <c r="FG151" s="5"/>
+      <c r="FH151" s="5"/>
+      <c r="FI151" s="5"/>
+      <c r="FJ151" s="5"/>
+      <c r="FK151" s="5"/>
+      <c r="FL151" s="5"/>
+      <c r="FM151" s="5"/>
+      <c r="FN151" s="5"/>
+      <c r="FO151" s="5"/>
+      <c r="FP151" s="5"/>
+      <c r="FQ151" s="5"/>
+      <c r="FR151" s="5"/>
+      <c r="FS151" s="5"/>
+      <c r="FT151" s="5"/>
+      <c r="FU151" s="5"/>
+      <c r="FV151" s="5"/>
+      <c r="FW151" s="5"/>
+      <c r="FX151" s="5"/>
+      <c r="FY151" s="5"/>
+      <c r="FZ151" s="5"/>
+      <c r="GA151" s="5"/>
+      <c r="GB151" s="5"/>
+      <c r="GC151" s="5"/>
+      <c r="GD151" s="5"/>
+      <c r="GE151" s="5"/>
+      <c r="GF151" s="5"/>
+      <c r="GG151" s="5"/>
+      <c r="GH151" s="5"/>
+      <c r="GI151" s="5"/>
+      <c r="GJ151" s="5"/>
+      <c r="GK151" s="5"/>
+      <c r="GL151" s="5"/>
+      <c r="GM151" s="5"/>
+      <c r="GN151" s="5"/>
+      <c r="GO151" s="5"/>
+      <c r="GP151" s="5"/>
+      <c r="GQ151" s="5"/>
+      <c r="GR151" s="5"/>
+      <c r="GS151" s="5"/>
+      <c r="GT151" s="5"/>
+      <c r="GU151" s="5"/>
+      <c r="GV151" s="5"/>
+      <c r="GW151" s="5"/>
+      <c r="GX151" s="5"/>
+      <c r="GY151" s="5"/>
+      <c r="GZ151" s="5"/>
+      <c r="HA151" s="5"/>
+      <c r="HB151" s="5"/>
+      <c r="HC151" s="5"/>
+      <c r="HD151" s="5"/>
+      <c r="HE151" s="5"/>
+      <c r="HF151" s="5"/>
+      <c r="HG151" s="5"/>
+      <c r="HH151" s="5"/>
+      <c r="HI151" s="5"/>
+      <c r="HJ151" s="5"/>
+      <c r="HK151" s="5"/>
+      <c r="HL151" s="5"/>
+      <c r="HM151" s="5"/>
+      <c r="HN151" s="5"/>
+      <c r="HO151" s="5"/>
+      <c r="HP151" s="5"/>
+      <c r="HQ151" s="5"/>
+      <c r="HR151" s="5"/>
+      <c r="HS151" s="5"/>
+      <c r="HT151" s="5"/>
+      <c r="HU151" s="5"/>
+      <c r="HV151" s="5"/>
+      <c r="HW151" s="5"/>
+      <c r="HX151" s="5"/>
+      <c r="HY151" s="5"/>
+      <c r="HZ151" s="5"/>
+      <c r="IA151" s="5"/>
+      <c r="IB151" s="5"/>
+      <c r="IC151" s="5"/>
+      <c r="ID151" s="5"/>
+      <c r="IE151" s="5"/>
+      <c r="IF151" s="5"/>
+      <c r="IG151" s="5"/>
+      <c r="IH151" s="5"/>
+      <c r="II151" s="5"/>
+      <c r="IJ151" s="5"/>
+      <c r="IK151" s="5"/>
+      <c r="IL151" s="5"/>
+      <c r="IM151" s="5"/>
+      <c r="IN151" s="5"/>
+      <c r="IO151" s="5"/>
+      <c r="IP151" s="5"/>
+      <c r="IQ151" s="5"/>
+      <c r="IR151" s="5"/>
+      <c r="IS151" s="5"/>
+      <c r="IT151" s="5"/>
+    </row>
+    <row r="152" spans="1:254" s="2" customFormat="1">
+      <c r="A152" s="4"/>
+      <c r="B152" s="4"/>
+      <c r="C152" s="4"/>
+      <c r="D152" s="4"/>
+      <c r="E152" s="4"/>
+      <c r="F152" s="4"/>
+      <c r="G152" s="34"/>
+      <c r="H152" s="4"/>
     </row>
     <row r="153" spans="1:254">
       <c r="A153" s="7"/>
-      <c r="B153" s="7"/>
+      <c r="B153" s="6"/>
       <c r="C153" s="7"/>
       <c r="D153" s="7"/>
       <c r="E153" s="7"/>
@@ -7223,7 +7323,7 @@
     </row>
     <row r="154" spans="1:254">
       <c r="A154" s="7"/>
-      <c r="B154" s="20"/>
+      <c r="B154" s="7"/>
       <c r="C154" s="7"/>
       <c r="D154" s="7"/>
       <c r="E154" s="7"/>
@@ -7233,7 +7333,7 @@
     </row>
     <row r="155" spans="1:254">
       <c r="A155" s="7"/>
-      <c r="B155" s="7"/>
+      <c r="B155" s="20"/>
       <c r="C155" s="7"/>
       <c r="D155" s="7"/>
       <c r="E155" s="7"/>
@@ -7244,7 +7344,7 @@
     <row r="156" spans="1:254">
       <c r="A156" s="7"/>
       <c r="B156" s="7"/>
-      <c r="C156" s="4"/>
+      <c r="C156" s="7"/>
       <c r="D156" s="7"/>
       <c r="E156" s="7"/>
       <c r="F156" s="7"/>
@@ -7284,7 +7384,7 @@
     <row r="160" spans="1:254">
       <c r="A160" s="7"/>
       <c r="B160" s="7"/>
-      <c r="C160" s="7"/>
+      <c r="C160" s="4"/>
       <c r="D160" s="7"/>
       <c r="E160" s="7"/>
       <c r="F160" s="7"/>
@@ -7293,7 +7393,7 @@
     </row>
     <row r="161" spans="1:8">
       <c r="A161" s="7"/>
-      <c r="B161" s="22"/>
+      <c r="B161" s="7"/>
       <c r="C161" s="7"/>
       <c r="D161" s="7"/>
       <c r="E161" s="7"/>
@@ -7313,7 +7413,7 @@
     </row>
     <row r="163" spans="1:8">
       <c r="A163" s="7"/>
-      <c r="B163" s="7"/>
+      <c r="B163" s="22"/>
       <c r="C163" s="7"/>
       <c r="D163" s="7"/>
       <c r="E163" s="7"/>
@@ -7323,7 +7423,7 @@
     </row>
     <row r="164" spans="1:8">
       <c r="A164" s="7"/>
-      <c r="B164" s="20"/>
+      <c r="B164" s="7"/>
       <c r="C164" s="7"/>
       <c r="D164" s="7"/>
       <c r="E164" s="7"/>
@@ -7343,7 +7443,7 @@
     </row>
     <row r="166" spans="1:8">
       <c r="A166" s="7"/>
-      <c r="B166" s="7"/>
+      <c r="B166" s="20"/>
       <c r="C166" s="7"/>
       <c r="D166" s="7"/>
       <c r="E166" s="7"/>
@@ -7363,7 +7463,7 @@
     </row>
     <row r="168" spans="1:8">
       <c r="A168" s="7"/>
-      <c r="B168" s="20"/>
+      <c r="B168" s="7"/>
       <c r="C168" s="7"/>
       <c r="D168" s="7"/>
       <c r="E168" s="7"/>
@@ -7383,7 +7483,7 @@
     </row>
     <row r="170" spans="1:8">
       <c r="A170" s="7"/>
-      <c r="B170" s="7"/>
+      <c r="B170" s="20"/>
       <c r="C170" s="7"/>
       <c r="D170" s="7"/>
       <c r="E170" s="7"/>
@@ -7403,7 +7503,7 @@
     </row>
     <row r="172" spans="1:8">
       <c r="A172" s="7"/>
-      <c r="B172" s="20"/>
+      <c r="B172" s="7"/>
       <c r="C172" s="7"/>
       <c r="D172" s="7"/>
       <c r="E172" s="7"/>
@@ -7423,7 +7523,7 @@
     </row>
     <row r="174" spans="1:8">
       <c r="A174" s="7"/>
-      <c r="B174" s="7"/>
+      <c r="B174" s="20"/>
       <c r="C174" s="7"/>
       <c r="D174" s="7"/>
       <c r="E174" s="7"/>
@@ -7463,7 +7563,7 @@
     </row>
     <row r="178" spans="1:8">
       <c r="A178" s="7"/>
-      <c r="B178" s="6"/>
+      <c r="B178" s="7"/>
       <c r="C178" s="7"/>
       <c r="D178" s="7"/>
       <c r="E178" s="7"/>
@@ -7473,8 +7573,8 @@
     </row>
     <row r="179" spans="1:8">
       <c r="A179" s="7"/>
-      <c r="B179" s="4"/>
-      <c r="C179" s="4"/>
+      <c r="B179" s="6"/>
+      <c r="C179" s="7"/>
       <c r="D179" s="7"/>
       <c r="E179" s="7"/>
       <c r="F179" s="7"/>
@@ -7483,7 +7583,7 @@
     </row>
     <row r="180" spans="1:8">
       <c r="A180" s="7"/>
-      <c r="B180" s="19"/>
+      <c r="B180" s="4"/>
       <c r="C180" s="4"/>
       <c r="D180" s="7"/>
       <c r="E180" s="7"/>
@@ -7553,7 +7653,7 @@
     </row>
     <row r="187" spans="1:8">
       <c r="A187" s="7"/>
-      <c r="B187" s="4"/>
+      <c r="B187" s="19"/>
       <c r="C187" s="4"/>
       <c r="D187" s="7"/>
       <c r="E187" s="7"/>
@@ -7563,7 +7663,7 @@
     </row>
     <row r="188" spans="1:8">
       <c r="A188" s="7"/>
-      <c r="B188" s="19"/>
+      <c r="B188" s="4"/>
       <c r="C188" s="4"/>
       <c r="D188" s="7"/>
       <c r="E188" s="7"/>
@@ -7573,7 +7673,7 @@
     </row>
     <row r="189" spans="1:8">
       <c r="A189" s="7"/>
-      <c r="B189" s="21"/>
+      <c r="B189" s="19"/>
       <c r="C189" s="4"/>
       <c r="D189" s="7"/>
       <c r="E189" s="7"/>
@@ -7593,7 +7693,7 @@
     </row>
     <row r="191" spans="1:8">
       <c r="A191" s="7"/>
-      <c r="B191" s="19"/>
+      <c r="B191" s="21"/>
       <c r="C191" s="4"/>
       <c r="D191" s="7"/>
       <c r="E191" s="7"/>
@@ -7634,7 +7734,7 @@
     <row r="195" spans="1:8">
       <c r="A195" s="7"/>
       <c r="B195" s="19"/>
-      <c r="C195" s="7"/>
+      <c r="C195" s="4"/>
       <c r="D195" s="7"/>
       <c r="E195" s="7"/>
       <c r="F195" s="7"/>
@@ -7643,7 +7743,7 @@
     </row>
     <row r="196" spans="1:8">
       <c r="A196" s="7"/>
-      <c r="B196" s="4"/>
+      <c r="B196" s="19"/>
       <c r="C196" s="7"/>
       <c r="D196" s="7"/>
       <c r="E196" s="7"/>
@@ -7663,7 +7763,7 @@
     </row>
     <row r="198" spans="1:8">
       <c r="A198" s="7"/>
-      <c r="B198" s="19"/>
+      <c r="B198" s="4"/>
       <c r="C198" s="7"/>
       <c r="D198" s="7"/>
       <c r="E198" s="7"/>
@@ -7723,7 +7823,7 @@
     </row>
     <row r="204" spans="1:8">
       <c r="A204" s="7"/>
-      <c r="B204" s="21"/>
+      <c r="B204" s="19"/>
       <c r="C204" s="7"/>
       <c r="D204" s="7"/>
       <c r="E204" s="7"/>
@@ -7763,7 +7863,7 @@
     </row>
     <row r="208" spans="1:8">
       <c r="A208" s="7"/>
-      <c r="B208" s="4"/>
+      <c r="B208" s="21"/>
       <c r="C208" s="7"/>
       <c r="D208" s="7"/>
       <c r="E208" s="7"/>
@@ -7773,7 +7873,7 @@
     </row>
     <row r="209" spans="1:8">
       <c r="A209" s="7"/>
-      <c r="B209" s="6"/>
+      <c r="B209" s="4"/>
       <c r="C209" s="7"/>
       <c r="D209" s="7"/>
       <c r="E209" s="7"/>
@@ -7783,7 +7883,7 @@
     </row>
     <row r="210" spans="1:8">
       <c r="A210" s="7"/>
-      <c r="B210" s="4"/>
+      <c r="B210" s="6"/>
       <c r="C210" s="7"/>
       <c r="D210" s="7"/>
       <c r="E210" s="7"/>
@@ -7793,7 +7893,7 @@
     </row>
     <row r="211" spans="1:8">
       <c r="A211" s="7"/>
-      <c r="B211" s="19"/>
+      <c r="B211" s="4"/>
       <c r="C211" s="7"/>
       <c r="D211" s="7"/>
       <c r="E211" s="7"/>
@@ -7843,7 +7943,7 @@
     </row>
     <row r="216" spans="1:8">
       <c r="A216" s="7"/>
-      <c r="B216" s="21"/>
+      <c r="B216" s="19"/>
       <c r="C216" s="7"/>
       <c r="D216" s="7"/>
       <c r="E216" s="7"/>
@@ -7853,7 +7953,7 @@
     </row>
     <row r="217" spans="1:8">
       <c r="A217" s="7"/>
-      <c r="B217" s="19"/>
+      <c r="B217" s="21"/>
       <c r="C217" s="7"/>
       <c r="D217" s="7"/>
       <c r="E217" s="7"/>
@@ -7903,7 +8003,7 @@
     </row>
     <row r="222" spans="1:8">
       <c r="A222" s="7"/>
-      <c r="B222" s="21"/>
+      <c r="B222" s="19"/>
       <c r="C222" s="7"/>
       <c r="D222" s="7"/>
       <c r="E222" s="7"/>
@@ -7963,7 +8063,7 @@
     </row>
     <row r="228" spans="1:8">
       <c r="A228" s="7"/>
-      <c r="B228" s="4"/>
+      <c r="B228" s="21"/>
       <c r="C228" s="7"/>
       <c r="D228" s="7"/>
       <c r="E228" s="7"/>
@@ -7973,7 +8073,7 @@
     </row>
     <row r="229" spans="1:8">
       <c r="A229" s="7"/>
-      <c r="B229" s="6"/>
+      <c r="B229" s="4"/>
       <c r="C229" s="7"/>
       <c r="D229" s="7"/>
       <c r="E229" s="7"/>
@@ -7983,8 +8083,8 @@
     </row>
     <row r="230" spans="1:8">
       <c r="A230" s="7"/>
-      <c r="B230" s="4"/>
-      <c r="C230" s="4"/>
+      <c r="B230" s="6"/>
+      <c r="C230" s="7"/>
       <c r="D230" s="7"/>
       <c r="E230" s="7"/>
       <c r="F230" s="7"/>
@@ -7993,7 +8093,7 @@
     </row>
     <row r="231" spans="1:8">
       <c r="A231" s="7"/>
-      <c r="B231" s="19"/>
+      <c r="B231" s="4"/>
       <c r="C231" s="4"/>
       <c r="D231" s="7"/>
       <c r="E231" s="7"/>
@@ -8003,7 +8103,7 @@
     </row>
     <row r="232" spans="1:8">
       <c r="A232" s="7"/>
-      <c r="B232" s="7"/>
+      <c r="B232" s="19"/>
       <c r="C232" s="4"/>
       <c r="D232" s="7"/>
       <c r="E232" s="7"/>
@@ -8013,7 +8113,7 @@
     </row>
     <row r="233" spans="1:8">
       <c r="A233" s="7"/>
-      <c r="B233" s="20"/>
+      <c r="B233" s="7"/>
       <c r="C233" s="4"/>
       <c r="D233" s="7"/>
       <c r="E233" s="7"/>
@@ -8053,7 +8153,7 @@
     </row>
     <row r="237" spans="1:8">
       <c r="A237" s="7"/>
-      <c r="B237" s="7"/>
+      <c r="B237" s="20"/>
       <c r="C237" s="4"/>
       <c r="D237" s="7"/>
       <c r="E237" s="7"/>
@@ -8063,7 +8163,7 @@
     </row>
     <row r="238" spans="1:8">
       <c r="A238" s="7"/>
-      <c r="B238" s="20"/>
+      <c r="B238" s="7"/>
       <c r="C238" s="4"/>
       <c r="D238" s="7"/>
       <c r="E238" s="7"/>
@@ -8073,7 +8173,7 @@
     </row>
     <row r="239" spans="1:8">
       <c r="A239" s="7"/>
-      <c r="B239" s="23"/>
+      <c r="B239" s="20"/>
       <c r="C239" s="4"/>
       <c r="D239" s="7"/>
       <c r="E239" s="7"/>
@@ -8093,7 +8193,7 @@
     </row>
     <row r="241" spans="1:8">
       <c r="A241" s="7"/>
-      <c r="B241" s="20"/>
+      <c r="B241" s="23"/>
       <c r="C241" s="4"/>
       <c r="D241" s="7"/>
       <c r="E241" s="7"/>
@@ -8133,7 +8233,7 @@
     </row>
     <row r="245" spans="1:8">
       <c r="A245" s="7"/>
-      <c r="B245" s="7"/>
+      <c r="B245" s="20"/>
       <c r="C245" s="4"/>
       <c r="D245" s="7"/>
       <c r="E245" s="7"/>
@@ -8143,7 +8243,7 @@
     </row>
     <row r="246" spans="1:8">
       <c r="A246" s="7"/>
-      <c r="B246" s="20"/>
+      <c r="B246" s="7"/>
       <c r="C246" s="4"/>
       <c r="D246" s="7"/>
       <c r="E246" s="7"/>
@@ -8193,7 +8293,7 @@
     </row>
     <row r="251" spans="1:8">
       <c r="A251" s="7"/>
-      <c r="B251" s="7"/>
+      <c r="B251" s="20"/>
       <c r="C251" s="4"/>
       <c r="D251" s="7"/>
       <c r="E251" s="7"/>
@@ -8203,8 +8303,8 @@
     </row>
     <row r="252" spans="1:8">
       <c r="A252" s="7"/>
-      <c r="B252" s="20"/>
-      <c r="C252" s="7"/>
+      <c r="B252" s="7"/>
+      <c r="C252" s="4"/>
       <c r="D252" s="7"/>
       <c r="E252" s="7"/>
       <c r="F252" s="7"/>
@@ -8213,7 +8313,7 @@
     </row>
     <row r="253" spans="1:8">
       <c r="A253" s="7"/>
-      <c r="B253" s="7"/>
+      <c r="B253" s="20"/>
       <c r="C253" s="7"/>
       <c r="D253" s="7"/>
       <c r="E253" s="7"/>
@@ -8223,7 +8323,7 @@
     </row>
     <row r="254" spans="1:8">
       <c r="A254" s="7"/>
-      <c r="B254" s="20"/>
+      <c r="B254" s="7"/>
       <c r="C254" s="7"/>
       <c r="D254" s="7"/>
       <c r="E254" s="7"/>
@@ -8233,7 +8333,7 @@
     </row>
     <row r="255" spans="1:8">
       <c r="A255" s="7"/>
-      <c r="B255" s="23"/>
+      <c r="B255" s="20"/>
       <c r="C255" s="7"/>
       <c r="D255" s="7"/>
       <c r="E255" s="7"/>
@@ -8283,8 +8383,8 @@
     </row>
     <row r="260" spans="1:8">
       <c r="A260" s="7"/>
-      <c r="B260" s="20"/>
-      <c r="C260" s="4"/>
+      <c r="B260" s="23"/>
+      <c r="C260" s="7"/>
       <c r="D260" s="7"/>
       <c r="E260" s="7"/>
       <c r="F260" s="7"/>
@@ -8293,7 +8393,7 @@
     </row>
     <row r="261" spans="1:8">
       <c r="A261" s="7"/>
-      <c r="B261" s="23"/>
+      <c r="B261" s="20"/>
       <c r="C261" s="4"/>
       <c r="D261" s="7"/>
       <c r="E261" s="7"/>
@@ -8303,7 +8403,7 @@
     </row>
     <row r="262" spans="1:8">
       <c r="A262" s="7"/>
-      <c r="B262" s="24"/>
+      <c r="B262" s="23"/>
       <c r="C262" s="4"/>
       <c r="D262" s="7"/>
       <c r="E262" s="7"/>
@@ -8331,9 +8431,9 @@
       <c r="G264" s="30"/>
       <c r="H264" s="7"/>
     </row>
-    <row r="265" spans="1:8" ht="11.25">
+    <row r="265" spans="1:8">
       <c r="A265" s="7"/>
-      <c r="B265" s="25"/>
+      <c r="B265" s="24"/>
       <c r="C265" s="4"/>
       <c r="D265" s="7"/>
       <c r="E265" s="7"/>
@@ -8341,9 +8441,9 @@
       <c r="G265" s="30"/>
       <c r="H265" s="7"/>
     </row>
-    <row r="266" spans="1:8">
+    <row r="266" spans="1:8" ht="11.25">
       <c r="A266" s="7"/>
-      <c r="B266" s="23"/>
+      <c r="B266" s="25"/>
       <c r="C266" s="4"/>
       <c r="D266" s="7"/>
       <c r="E266" s="7"/>
@@ -8383,7 +8483,7 @@
     </row>
     <row r="270" spans="1:8">
       <c r="A270" s="7"/>
-      <c r="B270" s="24"/>
+      <c r="B270" s="23"/>
       <c r="C270" s="4"/>
       <c r="D270" s="7"/>
       <c r="E270" s="7"/>
@@ -8413,7 +8513,7 @@
     </row>
     <row r="273" spans="1:8">
       <c r="A273" s="7"/>
-      <c r="B273" s="23"/>
+      <c r="B273" s="24"/>
       <c r="C273" s="4"/>
       <c r="D273" s="7"/>
       <c r="E273" s="7"/>
@@ -8423,7 +8523,7 @@
     </row>
     <row r="274" spans="1:8">
       <c r="A274" s="7"/>
-      <c r="B274" s="24"/>
+      <c r="B274" s="23"/>
       <c r="C274" s="4"/>
       <c r="D274" s="7"/>
       <c r="E274" s="7"/>
@@ -8431,15 +8531,15 @@
       <c r="G274" s="30"/>
       <c r="H274" s="7"/>
     </row>
-    <row r="275" spans="1:8" s="2" customFormat="1">
-      <c r="A275" s="4"/>
+    <row r="275" spans="1:8">
+      <c r="A275" s="7"/>
       <c r="B275" s="24"/>
       <c r="C275" s="4"/>
-      <c r="D275" s="4"/>
-      <c r="E275" s="4"/>
-      <c r="F275" s="4"/>
-      <c r="G275" s="34"/>
-      <c r="H275" s="4"/>
+      <c r="D275" s="7"/>
+      <c r="E275" s="7"/>
+      <c r="F275" s="7"/>
+      <c r="G275" s="30"/>
+      <c r="H275" s="7"/>
     </row>
     <row r="276" spans="1:8" s="2" customFormat="1">
       <c r="A276" s="4"/>
@@ -8451,19 +8551,19 @@
       <c r="G276" s="34"/>
       <c r="H276" s="4"/>
     </row>
-    <row r="277" spans="1:8">
-      <c r="A277" s="7"/>
+    <row r="277" spans="1:8" s="2" customFormat="1">
+      <c r="A277" s="4"/>
       <c r="B277" s="24"/>
       <c r="C277" s="4"/>
-      <c r="D277" s="7"/>
-      <c r="E277" s="7"/>
-      <c r="F277" s="7"/>
-      <c r="G277" s="30"/>
-      <c r="H277" s="7"/>
+      <c r="D277" s="4"/>
+      <c r="E277" s="4"/>
+      <c r="F277" s="4"/>
+      <c r="G277" s="34"/>
+      <c r="H277" s="4"/>
     </row>
     <row r="278" spans="1:8">
       <c r="A278" s="7"/>
-      <c r="B278" s="23"/>
+      <c r="B278" s="24"/>
       <c r="C278" s="4"/>
       <c r="D278" s="7"/>
       <c r="E278" s="7"/>
@@ -8473,7 +8573,7 @@
     </row>
     <row r="279" spans="1:8">
       <c r="A279" s="7"/>
-      <c r="B279" s="24"/>
+      <c r="B279" s="23"/>
       <c r="C279" s="4"/>
       <c r="D279" s="7"/>
       <c r="E279" s="7"/>
@@ -8503,7 +8603,7 @@
     </row>
     <row r="282" spans="1:8">
       <c r="A282" s="7"/>
-      <c r="B282" s="22"/>
+      <c r="B282" s="24"/>
       <c r="C282" s="4"/>
       <c r="D282" s="7"/>
       <c r="E282" s="7"/>
@@ -8513,7 +8613,7 @@
     </row>
     <row r="283" spans="1:8">
       <c r="A283" s="7"/>
-      <c r="B283" s="7"/>
+      <c r="B283" s="22"/>
       <c r="C283" s="4"/>
       <c r="D283" s="7"/>
       <c r="E283" s="7"/>
@@ -8533,7 +8633,7 @@
     </row>
     <row r="285" spans="1:8">
       <c r="A285" s="7"/>
-      <c r="B285" s="20"/>
+      <c r="B285" s="7"/>
       <c r="C285" s="4"/>
       <c r="D285" s="7"/>
       <c r="E285" s="7"/>
@@ -8553,7 +8653,7 @@
     </row>
     <row r="287" spans="1:8">
       <c r="A287" s="7"/>
-      <c r="B287" s="7"/>
+      <c r="B287" s="20"/>
       <c r="C287" s="4"/>
       <c r="D287" s="7"/>
       <c r="E287" s="7"/>
@@ -8584,7 +8684,7 @@
     <row r="290" spans="1:8">
       <c r="A290" s="7"/>
       <c r="B290" s="7"/>
-      <c r="C290" s="7"/>
+      <c r="C290" s="4"/>
       <c r="D290" s="7"/>
       <c r="E290" s="7"/>
       <c r="F290" s="7"/>
@@ -8593,7 +8693,7 @@
     </row>
     <row r="291" spans="1:8">
       <c r="A291" s="7"/>
-      <c r="B291" s="6"/>
+      <c r="B291" s="7"/>
       <c r="C291" s="7"/>
       <c r="D291" s="7"/>
       <c r="E291" s="7"/>
@@ -8603,7 +8703,7 @@
     </row>
     <row r="292" spans="1:8">
       <c r="A292" s="7"/>
-      <c r="B292" s="7"/>
+      <c r="B292" s="6"/>
       <c r="C292" s="7"/>
       <c r="D292" s="7"/>
       <c r="E292" s="7"/>
@@ -8683,7 +8783,7 @@
     </row>
     <row r="300" spans="1:8">
       <c r="A300" s="7"/>
-      <c r="B300" s="6"/>
+      <c r="B300" s="7"/>
       <c r="C300" s="7"/>
       <c r="D300" s="7"/>
       <c r="E300" s="7"/>
@@ -8693,8 +8793,8 @@
     </row>
     <row r="301" spans="1:8">
       <c r="A301" s="7"/>
-      <c r="B301" s="4"/>
-      <c r="C301" s="4"/>
+      <c r="B301" s="6"/>
+      <c r="C301" s="7"/>
       <c r="D301" s="7"/>
       <c r="E301" s="7"/>
       <c r="F301" s="7"/>
@@ -8703,7 +8803,7 @@
     </row>
     <row r="302" spans="1:8">
       <c r="A302" s="7"/>
-      <c r="B302" s="19"/>
+      <c r="B302" s="4"/>
       <c r="C302" s="4"/>
       <c r="D302" s="7"/>
       <c r="E302" s="7"/>
@@ -8733,7 +8833,7 @@
     </row>
     <row r="305" spans="1:8">
       <c r="A305" s="7"/>
-      <c r="B305" s="4"/>
+      <c r="B305" s="19"/>
       <c r="C305" s="4"/>
       <c r="D305" s="7"/>
       <c r="E305" s="7"/>
@@ -8793,7 +8893,7 @@
     </row>
     <row r="311" spans="1:8">
       <c r="A311" s="7"/>
-      <c r="B311" s="19"/>
+      <c r="B311" s="4"/>
       <c r="C311" s="4"/>
       <c r="D311" s="7"/>
       <c r="E311" s="7"/>
@@ -8813,7 +8913,7 @@
     </row>
     <row r="313" spans="1:8">
       <c r="A313" s="7"/>
-      <c r="B313" s="21"/>
+      <c r="B313" s="19"/>
       <c r="C313" s="4"/>
       <c r="D313" s="7"/>
       <c r="E313" s="7"/>
@@ -8823,8 +8923,8 @@
     </row>
     <row r="314" spans="1:8">
       <c r="A314" s="7"/>
-      <c r="B314" s="7"/>
-      <c r="C314" s="7"/>
+      <c r="B314" s="21"/>
+      <c r="C314" s="4"/>
       <c r="D314" s="7"/>
       <c r="E314" s="7"/>
       <c r="F314" s="7"/>
@@ -8833,7 +8933,7 @@
     </row>
     <row r="315" spans="1:8">
       <c r="A315" s="7"/>
-      <c r="B315" s="6"/>
+      <c r="B315" s="7"/>
       <c r="C315" s="7"/>
       <c r="D315" s="7"/>
       <c r="E315" s="7"/>
@@ -8841,15 +8941,15 @@
       <c r="G315" s="30"/>
       <c r="H315" s="7"/>
     </row>
-    <row r="316" spans="1:8" s="2" customFormat="1">
-      <c r="A316" s="4"/>
-      <c r="B316" s="4"/>
-      <c r="C316" s="9"/>
-      <c r="D316" s="4"/>
-      <c r="E316" s="4"/>
-      <c r="F316" s="4"/>
-      <c r="G316" s="34"/>
-      <c r="H316" s="4"/>
+    <row r="316" spans="1:8">
+      <c r="A316" s="7"/>
+      <c r="B316" s="6"/>
+      <c r="C316" s="7"/>
+      <c r="D316" s="7"/>
+      <c r="E316" s="7"/>
+      <c r="F316" s="7"/>
+      <c r="G316" s="30"/>
+      <c r="H316" s="7"/>
     </row>
     <row r="317" spans="1:8" s="2" customFormat="1">
       <c r="A317" s="4"/>
@@ -8873,7 +8973,7 @@
     </row>
     <row r="319" spans="1:8" s="2" customFormat="1">
       <c r="A319" s="4"/>
-      <c r="B319" s="19"/>
+      <c r="B319" s="4"/>
       <c r="C319" s="9"/>
       <c r="D319" s="4"/>
       <c r="E319" s="4"/>
@@ -8923,8 +9023,8 @@
     </row>
     <row r="324" spans="1:8" s="2" customFormat="1">
       <c r="A324" s="4"/>
-      <c r="B324" s="26"/>
-      <c r="C324" s="4"/>
+      <c r="B324" s="19"/>
+      <c r="C324" s="9"/>
       <c r="D324" s="4"/>
       <c r="E324" s="4"/>
       <c r="F324" s="4"/>
@@ -8973,7 +9073,7 @@
     </row>
     <row r="329" spans="1:8" s="2" customFormat="1">
       <c r="A329" s="4"/>
-      <c r="B329" s="21"/>
+      <c r="B329" s="26"/>
       <c r="C329" s="4"/>
       <c r="D329" s="4"/>
       <c r="E329" s="4"/>
@@ -9023,7 +9123,7 @@
     </row>
     <row r="334" spans="1:8" s="2" customFormat="1">
       <c r="A334" s="4"/>
-      <c r="B334" s="19"/>
+      <c r="B334" s="21"/>
       <c r="C334" s="4"/>
       <c r="D334" s="4"/>
       <c r="E334" s="4"/>
@@ -9033,7 +9133,7 @@
     </row>
     <row r="335" spans="1:8" s="2" customFormat="1">
       <c r="A335" s="4"/>
-      <c r="B335" s="21"/>
+      <c r="B335" s="19"/>
       <c r="C335" s="4"/>
       <c r="D335" s="4"/>
       <c r="E335" s="4"/>
@@ -9043,7 +9143,7 @@
     </row>
     <row r="336" spans="1:8" s="2" customFormat="1">
       <c r="A336" s="4"/>
-      <c r="B336" s="4"/>
+      <c r="B336" s="21"/>
       <c r="C336" s="4"/>
       <c r="D336" s="4"/>
       <c r="E336" s="4"/>
@@ -9051,20 +9151,20 @@
       <c r="G336" s="34"/>
       <c r="H336" s="4"/>
     </row>
-    <row r="337" spans="1:8">
-      <c r="A337" s="7"/>
-      <c r="B337" s="6"/>
-      <c r="C337" s="7"/>
-      <c r="D337" s="7"/>
-      <c r="E337" s="7"/>
-      <c r="F337" s="7"/>
-      <c r="G337" s="30"/>
-      <c r="H337" s="7"/>
+    <row r="337" spans="1:8" s="2" customFormat="1">
+      <c r="A337" s="4"/>
+      <c r="B337" s="4"/>
+      <c r="C337" s="4"/>
+      <c r="D337" s="4"/>
+      <c r="E337" s="4"/>
+      <c r="F337" s="4"/>
+      <c r="G337" s="34"/>
+      <c r="H337" s="4"/>
     </row>
     <row r="338" spans="1:8">
       <c r="A338" s="7"/>
-      <c r="B338" s="7"/>
-      <c r="C338" s="4"/>
+      <c r="B338" s="6"/>
+      <c r="C338" s="7"/>
       <c r="D338" s="7"/>
       <c r="E338" s="7"/>
       <c r="F338" s="7"/>
@@ -9133,7 +9233,7 @@
     </row>
     <row r="345" spans="1:8">
       <c r="A345" s="7"/>
-      <c r="B345" s="4"/>
+      <c r="B345" s="7"/>
       <c r="C345" s="4"/>
       <c r="D345" s="7"/>
       <c r="E345" s="7"/>
@@ -9144,7 +9244,7 @@
     <row r="346" spans="1:8">
       <c r="A346" s="7"/>
       <c r="B346" s="4"/>
-      <c r="C346" s="7"/>
+      <c r="C346" s="4"/>
       <c r="D346" s="7"/>
       <c r="E346" s="7"/>
       <c r="F346" s="7"/>
@@ -9153,7 +9253,7 @@
     </row>
     <row r="347" spans="1:8">
       <c r="A347" s="7"/>
-      <c r="B347" s="6"/>
+      <c r="B347" s="4"/>
       <c r="C347" s="7"/>
       <c r="D347" s="7"/>
       <c r="E347" s="7"/>
@@ -9163,7 +9263,7 @@
     </row>
     <row r="348" spans="1:8">
       <c r="A348" s="7"/>
-      <c r="B348" s="7"/>
+      <c r="B348" s="6"/>
       <c r="C348" s="7"/>
       <c r="D348" s="7"/>
       <c r="E348" s="7"/>
@@ -9173,7 +9273,7 @@
     </row>
     <row r="349" spans="1:8">
       <c r="A349" s="7"/>
-      <c r="B349" s="22"/>
+      <c r="B349" s="7"/>
       <c r="C349" s="7"/>
       <c r="D349" s="7"/>
       <c r="E349" s="7"/>
@@ -9183,7 +9283,7 @@
     </row>
     <row r="350" spans="1:8">
       <c r="A350" s="7"/>
-      <c r="B350" s="7"/>
+      <c r="B350" s="22"/>
       <c r="C350" s="7"/>
       <c r="D350" s="7"/>
       <c r="E350" s="7"/>
@@ -9223,7 +9323,7 @@
     </row>
     <row r="354" spans="1:8">
       <c r="A354" s="7"/>
-      <c r="B354" s="6"/>
+      <c r="B354" s="7"/>
       <c r="C354" s="7"/>
       <c r="D354" s="7"/>
       <c r="E354" s="7"/>
@@ -9233,7 +9333,7 @@
     </row>
     <row r="355" spans="1:8">
       <c r="A355" s="7"/>
-      <c r="B355" s="7"/>
+      <c r="B355" s="6"/>
       <c r="C355" s="7"/>
       <c r="D355" s="7"/>
       <c r="E355" s="7"/>
@@ -9243,7 +9343,7 @@
     </row>
     <row r="356" spans="1:8">
       <c r="A356" s="7"/>
-      <c r="B356" s="20"/>
+      <c r="B356" s="7"/>
       <c r="C356" s="7"/>
       <c r="D356" s="7"/>
       <c r="E356" s="7"/>
@@ -9273,7 +9373,7 @@
     </row>
     <row r="359" spans="1:8">
       <c r="A359" s="7"/>
-      <c r="B359" s="22"/>
+      <c r="B359" s="20"/>
       <c r="C359" s="7"/>
       <c r="D359" s="7"/>
       <c r="E359" s="7"/>
@@ -9283,7 +9383,7 @@
     </row>
     <row r="360" spans="1:8">
       <c r="A360" s="7"/>
-      <c r="B360" s="20"/>
+      <c r="B360" s="22"/>
       <c r="C360" s="7"/>
       <c r="D360" s="7"/>
       <c r="E360" s="7"/>
@@ -9303,7 +9403,7 @@
     </row>
     <row r="362" spans="1:8">
       <c r="A362" s="7"/>
-      <c r="B362" s="22"/>
+      <c r="B362" s="20"/>
       <c r="C362" s="7"/>
       <c r="D362" s="7"/>
       <c r="E362" s="7"/>
@@ -9313,7 +9413,7 @@
     </row>
     <row r="363" spans="1:8">
       <c r="A363" s="7"/>
-      <c r="B363" s="20"/>
+      <c r="B363" s="22"/>
       <c r="C363" s="7"/>
       <c r="D363" s="7"/>
       <c r="E363" s="7"/>
@@ -9323,7 +9423,7 @@
     </row>
     <row r="364" spans="1:8">
       <c r="A364" s="7"/>
-      <c r="B364" s="22"/>
+      <c r="B364" s="20"/>
       <c r="C364" s="7"/>
       <c r="D364" s="7"/>
       <c r="E364" s="7"/>
@@ -9333,7 +9433,7 @@
     </row>
     <row r="365" spans="1:8">
       <c r="A365" s="7"/>
-      <c r="B365" s="20"/>
+      <c r="B365" s="22"/>
       <c r="C365" s="7"/>
       <c r="D365" s="7"/>
       <c r="E365" s="7"/>
@@ -9363,7 +9463,7 @@
     </row>
     <row r="368" spans="1:8">
       <c r="A368" s="7"/>
-      <c r="B368" s="7"/>
+      <c r="B368" s="20"/>
       <c r="C368" s="7"/>
       <c r="D368" s="7"/>
       <c r="E368" s="7"/>
@@ -9373,7 +9473,7 @@
     </row>
     <row r="369" spans="1:8">
       <c r="A369" s="7"/>
-      <c r="B369" s="27"/>
+      <c r="B369" s="7"/>
       <c r="C369" s="7"/>
       <c r="D369" s="7"/>
       <c r="E369" s="7"/>
@@ -9383,7 +9483,7 @@
     </row>
     <row r="370" spans="1:8">
       <c r="A370" s="7"/>
-      <c r="B370" s="22"/>
+      <c r="B370" s="27"/>
       <c r="C370" s="7"/>
       <c r="D370" s="7"/>
       <c r="E370" s="7"/>
@@ -9393,8 +9493,8 @@
     </row>
     <row r="371" spans="1:8">
       <c r="A371" s="7"/>
-      <c r="B371" s="7"/>
-      <c r="C371" s="4"/>
+      <c r="B371" s="22"/>
+      <c r="C371" s="7"/>
       <c r="D371" s="7"/>
       <c r="E371" s="7"/>
       <c r="F371" s="7"/>
@@ -9403,7 +9503,7 @@
     </row>
     <row r="372" spans="1:8">
       <c r="A372" s="7"/>
-      <c r="B372" s="20"/>
+      <c r="B372" s="7"/>
       <c r="C372" s="4"/>
       <c r="D372" s="7"/>
       <c r="E372" s="7"/>
@@ -9433,7 +9533,7 @@
     </row>
     <row r="375" spans="1:8">
       <c r="A375" s="7"/>
-      <c r="B375" s="7"/>
+      <c r="B375" s="20"/>
       <c r="C375" s="4"/>
       <c r="D375" s="7"/>
       <c r="E375" s="7"/>
@@ -9463,7 +9563,7 @@
     </row>
     <row r="378" spans="1:8">
       <c r="A378" s="7"/>
-      <c r="B378" s="20"/>
+      <c r="B378" s="7"/>
       <c r="C378" s="4"/>
       <c r="D378" s="7"/>
       <c r="E378" s="7"/>
@@ -9483,8 +9583,8 @@
     </row>
     <row r="380" spans="1:8">
       <c r="A380" s="7"/>
-      <c r="B380" s="7"/>
-      <c r="C380" s="7"/>
+      <c r="B380" s="20"/>
+      <c r="C380" s="4"/>
       <c r="D380" s="7"/>
       <c r="E380" s="7"/>
       <c r="F380" s="7"/>
@@ -9493,7 +9593,7 @@
     </row>
     <row r="381" spans="1:8">
       <c r="A381" s="7"/>
-      <c r="B381" s="6"/>
+      <c r="B381" s="7"/>
       <c r="C381" s="7"/>
       <c r="D381" s="7"/>
       <c r="E381" s="7"/>
@@ -9503,7 +9603,7 @@
     </row>
     <row r="382" spans="1:8">
       <c r="A382" s="7"/>
-      <c r="B382" s="7"/>
+      <c r="B382" s="6"/>
       <c r="C382" s="7"/>
       <c r="D382" s="7"/>
       <c r="E382" s="7"/>
@@ -9563,7 +9663,7 @@
     </row>
     <row r="388" spans="1:8">
       <c r="A388" s="7"/>
-      <c r="B388" s="6"/>
+      <c r="B388" s="7"/>
       <c r="C388" s="7"/>
       <c r="D388" s="7"/>
       <c r="E388" s="7"/>
@@ -9573,7 +9673,7 @@
     </row>
     <row r="389" spans="1:8">
       <c r="A389" s="7"/>
-      <c r="B389" s="7"/>
+      <c r="B389" s="6"/>
       <c r="C389" s="7"/>
       <c r="D389" s="7"/>
       <c r="E389" s="7"/>
@@ -9594,7 +9694,7 @@
     <row r="391" spans="1:8">
       <c r="A391" s="7"/>
       <c r="B391" s="7"/>
-      <c r="C391" s="4"/>
+      <c r="C391" s="7"/>
       <c r="D391" s="7"/>
       <c r="E391" s="7"/>
       <c r="F391" s="7"/>
@@ -9603,7 +9703,7 @@
     </row>
     <row r="392" spans="1:8">
       <c r="A392" s="7"/>
-      <c r="B392" s="20"/>
+      <c r="B392" s="7"/>
       <c r="C392" s="4"/>
       <c r="D392" s="7"/>
       <c r="E392" s="7"/>
@@ -9614,7 +9714,7 @@
     <row r="393" spans="1:8">
       <c r="A393" s="7"/>
       <c r="B393" s="20"/>
-      <c r="C393" s="7"/>
+      <c r="C393" s="4"/>
       <c r="D393" s="7"/>
       <c r="E393" s="7"/>
       <c r="F393" s="7"/>
@@ -9623,7 +9723,7 @@
     </row>
     <row r="394" spans="1:8">
       <c r="A394" s="7"/>
-      <c r="B394" s="27"/>
+      <c r="B394" s="20"/>
       <c r="C394" s="7"/>
       <c r="D394" s="7"/>
       <c r="E394" s="7"/>
@@ -9633,7 +9733,7 @@
     </row>
     <row r="395" spans="1:8">
       <c r="A395" s="7"/>
-      <c r="B395" s="22"/>
+      <c r="B395" s="27"/>
       <c r="C395" s="7"/>
       <c r="D395" s="7"/>
       <c r="E395" s="7"/>
@@ -9683,7 +9783,7 @@
     </row>
     <row r="400" spans="1:8">
       <c r="A400" s="7"/>
-      <c r="B400" s="7"/>
+      <c r="B400" s="22"/>
       <c r="C400" s="7"/>
       <c r="D400" s="7"/>
       <c r="E400" s="7"/>
@@ -9693,7 +9793,7 @@
     </row>
     <row r="401" spans="1:8">
       <c r="A401" s="7"/>
-      <c r="B401" s="6"/>
+      <c r="B401" s="7"/>
       <c r="C401" s="7"/>
       <c r="D401" s="7"/>
       <c r="E401" s="7"/>
@@ -9703,7 +9803,7 @@
     </row>
     <row r="402" spans="1:8">
       <c r="A402" s="7"/>
-      <c r="B402" s="7"/>
+      <c r="B402" s="6"/>
       <c r="C402" s="7"/>
       <c r="D402" s="7"/>
       <c r="E402" s="7"/>
@@ -9713,7 +9813,7 @@
     </row>
     <row r="403" spans="1:8">
       <c r="A403" s="7"/>
-      <c r="B403" s="20"/>
+      <c r="B403" s="7"/>
       <c r="C403" s="7"/>
       <c r="D403" s="7"/>
       <c r="E403" s="7"/>
@@ -9723,7 +9823,7 @@
     </row>
     <row r="404" spans="1:8">
       <c r="A404" s="7"/>
-      <c r="B404" s="22"/>
+      <c r="B404" s="20"/>
       <c r="C404" s="7"/>
       <c r="D404" s="7"/>
       <c r="E404" s="7"/>
@@ -9743,7 +9843,7 @@
     </row>
     <row r="406" spans="1:8">
       <c r="A406" s="7"/>
-      <c r="B406" s="20"/>
+      <c r="B406" s="22"/>
       <c r="C406" s="7"/>
       <c r="D406" s="7"/>
       <c r="E406" s="7"/>
@@ -9783,7 +9883,7 @@
     </row>
     <row r="410" spans="1:8">
       <c r="A410" s="7"/>
-      <c r="B410" s="7"/>
+      <c r="B410" s="20"/>
       <c r="C410" s="7"/>
       <c r="D410" s="7"/>
       <c r="E410" s="7"/>
@@ -9793,7 +9893,7 @@
     </row>
     <row r="411" spans="1:8">
       <c r="A411" s="7"/>
-      <c r="B411" s="20"/>
+      <c r="B411" s="7"/>
       <c r="C411" s="7"/>
       <c r="D411" s="7"/>
       <c r="E411" s="7"/>
@@ -9813,7 +9913,7 @@
     </row>
     <row r="413" spans="1:8">
       <c r="A413" s="7"/>
-      <c r="B413" s="22"/>
+      <c r="B413" s="20"/>
       <c r="C413" s="7"/>
       <c r="D413" s="7"/>
       <c r="E413" s="7"/>
@@ -9823,7 +9923,7 @@
     </row>
     <row r="414" spans="1:8">
       <c r="A414" s="7"/>
-      <c r="B414" s="7"/>
+      <c r="B414" s="22"/>
       <c r="C414" s="7"/>
       <c r="D414" s="7"/>
       <c r="E414" s="7"/>
@@ -9833,7 +9933,7 @@
     </row>
     <row r="415" spans="1:8">
       <c r="A415" s="7"/>
-      <c r="B415" s="6"/>
+      <c r="B415" s="7"/>
       <c r="C415" s="7"/>
       <c r="D415" s="7"/>
       <c r="E415" s="7"/>
@@ -9843,7 +9943,7 @@
     </row>
     <row r="416" spans="1:8">
       <c r="A416" s="7"/>
-      <c r="B416" s="7"/>
+      <c r="B416" s="6"/>
       <c r="C416" s="7"/>
       <c r="D416" s="7"/>
       <c r="E416" s="7"/>
@@ -9863,7 +9963,7 @@
     </row>
     <row r="418" spans="1:8">
       <c r="A418" s="7"/>
-      <c r="B418" s="6"/>
+      <c r="B418" s="7"/>
       <c r="C418" s="7"/>
       <c r="D418" s="7"/>
       <c r="E418" s="7"/>
@@ -9873,7 +9973,7 @@
     </row>
     <row r="419" spans="1:8">
       <c r="A419" s="7"/>
-      <c r="B419" s="7"/>
+      <c r="B419" s="6"/>
       <c r="C419" s="7"/>
       <c r="D419" s="7"/>
       <c r="E419" s="7"/>
@@ -9883,7 +9983,7 @@
     </row>
     <row r="420" spans="1:8">
       <c r="A420" s="7"/>
-      <c r="B420" s="20"/>
+      <c r="B420" s="7"/>
       <c r="C420" s="7"/>
       <c r="D420" s="7"/>
       <c r="E420" s="7"/>
@@ -9903,7 +10003,7 @@
     </row>
     <row r="422" spans="1:8">
       <c r="A422" s="7"/>
-      <c r="B422" s="7"/>
+      <c r="B422" s="20"/>
       <c r="C422" s="7"/>
       <c r="D422" s="7"/>
       <c r="E422" s="7"/>
@@ -9913,7 +10013,7 @@
     </row>
     <row r="423" spans="1:8">
       <c r="A423" s="7"/>
-      <c r="B423" s="6"/>
+      <c r="B423" s="7"/>
       <c r="C423" s="7"/>
       <c r="D423" s="7"/>
       <c r="E423" s="7"/>
@@ -9923,7 +10023,7 @@
     </row>
     <row r="424" spans="1:8">
       <c r="A424" s="7"/>
-      <c r="B424" s="7"/>
+      <c r="B424" s="6"/>
       <c r="C424" s="7"/>
       <c r="D424" s="7"/>
       <c r="E424" s="7"/>
@@ -9973,7 +10073,7 @@
     </row>
     <row r="429" spans="1:8">
       <c r="A429" s="7"/>
-      <c r="B429" s="6"/>
+      <c r="B429" s="7"/>
       <c r="C429" s="7"/>
       <c r="D429" s="7"/>
       <c r="E429" s="7"/>
@@ -9983,7 +10083,7 @@
     </row>
     <row r="430" spans="1:8">
       <c r="A430" s="7"/>
-      <c r="B430" s="7"/>
+      <c r="B430" s="6"/>
       <c r="C430" s="7"/>
       <c r="D430" s="7"/>
       <c r="E430" s="7"/>
@@ -10043,7 +10143,7 @@
     </row>
     <row r="436" spans="1:8">
       <c r="A436" s="7"/>
-      <c r="B436" s="6"/>
+      <c r="B436" s="7"/>
       <c r="C436" s="7"/>
       <c r="D436" s="7"/>
       <c r="E436" s="7"/>
@@ -10053,7 +10153,7 @@
     </row>
     <row r="437" spans="1:8">
       <c r="A437" s="7"/>
-      <c r="B437" s="7"/>
+      <c r="B437" s="6"/>
       <c r="C437" s="7"/>
       <c r="D437" s="7"/>
       <c r="E437" s="7"/>
@@ -10073,7 +10173,7 @@
     </row>
     <row r="439" spans="1:8">
       <c r="A439" s="7"/>
-      <c r="B439" s="6"/>
+      <c r="B439" s="7"/>
       <c r="C439" s="7"/>
       <c r="D439" s="7"/>
       <c r="E439" s="7"/>
@@ -10083,7 +10183,7 @@
     </row>
     <row r="440" spans="1:8">
       <c r="A440" s="7"/>
-      <c r="B440" s="4"/>
+      <c r="B440" s="6"/>
       <c r="C440" s="7"/>
       <c r="D440" s="7"/>
       <c r="E440" s="7"/>
@@ -10103,7 +10203,7 @@
     </row>
     <row r="442" spans="1:8">
       <c r="A442" s="7"/>
-      <c r="B442" s="7"/>
+      <c r="B442" s="4"/>
       <c r="C442" s="7"/>
       <c r="D442" s="7"/>
       <c r="E442" s="7"/>
@@ -10133,7 +10233,7 @@
     </row>
     <row r="445" spans="1:8">
       <c r="A445" s="7"/>
-      <c r="B445" s="6"/>
+      <c r="B445" s="7"/>
       <c r="C445" s="7"/>
       <c r="D445" s="7"/>
       <c r="E445" s="7"/>
@@ -10143,8 +10243,8 @@
     </row>
     <row r="446" spans="1:8">
       <c r="A446" s="7"/>
-      <c r="B446" s="7"/>
-      <c r="C446" s="4"/>
+      <c r="B446" s="6"/>
+      <c r="C446" s="7"/>
       <c r="D446" s="7"/>
       <c r="E446" s="7"/>
       <c r="F446" s="7"/>
@@ -10194,7 +10294,7 @@
     <row r="451" spans="1:8">
       <c r="A451" s="7"/>
       <c r="B451" s="7"/>
-      <c r="C451" s="7"/>
+      <c r="C451" s="4"/>
       <c r="D451" s="7"/>
       <c r="E451" s="7"/>
       <c r="F451" s="7"/>
@@ -10203,7 +10303,7 @@
     </row>
     <row r="452" spans="1:8">
       <c r="A452" s="7"/>
-      <c r="B452" s="6"/>
+      <c r="B452" s="7"/>
       <c r="C452" s="7"/>
       <c r="D452" s="7"/>
       <c r="E452" s="7"/>
@@ -10213,8 +10313,8 @@
     </row>
     <row r="453" spans="1:8">
       <c r="A453" s="7"/>
-      <c r="B453" s="7"/>
-      <c r="C453" s="4"/>
+      <c r="B453" s="6"/>
+      <c r="C453" s="7"/>
       <c r="D453" s="7"/>
       <c r="E453" s="7"/>
       <c r="F453" s="7"/>
@@ -10254,7 +10354,7 @@
     <row r="457" spans="1:8">
       <c r="A457" s="7"/>
       <c r="B457" s="7"/>
-      <c r="C457" s="7"/>
+      <c r="C457" s="4"/>
       <c r="D457" s="7"/>
       <c r="E457" s="7"/>
       <c r="F457" s="7"/>
@@ -10263,7 +10363,7 @@
     </row>
     <row r="458" spans="1:8">
       <c r="A458" s="7"/>
-      <c r="B458" s="6"/>
+      <c r="B458" s="7"/>
       <c r="C458" s="7"/>
       <c r="D458" s="7"/>
       <c r="E458" s="7"/>
@@ -10273,7 +10373,7 @@
     </row>
     <row r="459" spans="1:8">
       <c r="A459" s="7"/>
-      <c r="B459" s="22"/>
+      <c r="B459" s="6"/>
       <c r="C459" s="7"/>
       <c r="D459" s="7"/>
       <c r="E459" s="7"/>
@@ -10333,7 +10433,7 @@
     </row>
     <row r="465" spans="1:8">
       <c r="A465" s="7"/>
-      <c r="B465" s="7"/>
+      <c r="B465" s="22"/>
       <c r="C465" s="7"/>
       <c r="D465" s="7"/>
       <c r="E465" s="7"/>
@@ -10343,7 +10443,7 @@
     </row>
     <row r="466" spans="1:8">
       <c r="A466" s="7"/>
-      <c r="B466" s="6"/>
+      <c r="B466" s="7"/>
       <c r="C466" s="7"/>
       <c r="D466" s="7"/>
       <c r="E466" s="7"/>
@@ -10353,7 +10453,7 @@
     </row>
     <row r="467" spans="1:8">
       <c r="A467" s="7"/>
-      <c r="B467" s="22"/>
+      <c r="B467" s="6"/>
       <c r="C467" s="7"/>
       <c r="D467" s="7"/>
       <c r="E467" s="7"/>
@@ -10382,8 +10482,8 @@
       <c r="H469" s="7"/>
     </row>
     <row r="470" spans="1:8">
-      <c r="A470" s="6"/>
-      <c r="B470" s="7"/>
+      <c r="A470" s="7"/>
+      <c r="B470" s="22"/>
       <c r="C470" s="7"/>
       <c r="D470" s="7"/>
       <c r="E470" s="7"/>
@@ -10392,7 +10492,7 @@
       <c r="H470" s="7"/>
     </row>
     <row r="471" spans="1:8">
-      <c r="A471" s="7"/>
+      <c r="A471" s="6"/>
       <c r="B471" s="7"/>
       <c r="C471" s="7"/>
       <c r="D471" s="7"/>
@@ -10433,7 +10533,7 @@
     </row>
     <row r="475" spans="1:8">
       <c r="A475" s="7"/>
-      <c r="B475" s="28"/>
+      <c r="B475" s="7"/>
       <c r="C475" s="7"/>
       <c r="D475" s="7"/>
       <c r="E475" s="7"/>
@@ -10463,7 +10563,7 @@
     </row>
     <row r="478" spans="1:8">
       <c r="A478" s="7"/>
-      <c r="B478" s="7"/>
+      <c r="B478" s="28"/>
       <c r="C478" s="7"/>
       <c r="D478" s="7"/>
       <c r="E478" s="7"/>
@@ -10473,7 +10573,7 @@
     </row>
     <row r="479" spans="1:8">
       <c r="A479" s="7"/>
-      <c r="B479" s="28"/>
+      <c r="B479" s="7"/>
       <c r="C479" s="7"/>
       <c r="D479" s="7"/>
       <c r="E479" s="7"/>
@@ -10483,7 +10583,7 @@
     </row>
     <row r="480" spans="1:8">
       <c r="A480" s="7"/>
-      <c r="B480" s="7"/>
+      <c r="B480" s="28"/>
       <c r="C480" s="7"/>
       <c r="D480" s="7"/>
       <c r="E480" s="7"/>
@@ -10493,21 +10593,21 @@
     </row>
     <row r="481" spans="1:8">
       <c r="A481" s="7"/>
-      <c r="B481" s="29"/>
-      <c r="C481" s="30"/>
+      <c r="B481" s="7"/>
+      <c r="C481" s="7"/>
       <c r="D481" s="7"/>
       <c r="E481" s="7"/>
-      <c r="F481" s="29"/>
+      <c r="F481" s="7"/>
       <c r="G481" s="30"/>
       <c r="H481" s="7"/>
     </row>
     <row r="482" spans="1:8">
       <c r="A482" s="7"/>
-      <c r="B482" s="7"/>
-      <c r="C482" s="7"/>
+      <c r="B482" s="29"/>
+      <c r="C482" s="30"/>
       <c r="D482" s="7"/>
       <c r="E482" s="7"/>
-      <c r="F482" s="7"/>
+      <c r="F482" s="29"/>
       <c r="G482" s="30"/>
       <c r="H482" s="7"/>
     </row>
@@ -14411,6 +14511,16 @@
       <c r="G872" s="30"/>
       <c r="H872" s="7"/>
     </row>
+    <row r="873" spans="1:8">
+      <c r="A873" s="7"/>
+      <c r="B873" s="7"/>
+      <c r="C873" s="7"/>
+      <c r="D873" s="7"/>
+      <c r="E873" s="7"/>
+      <c r="F873" s="7"/>
+      <c r="G873" s="30"/>
+      <c r="H873" s="7"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>